<commit_message>
oppdatert, hvordan velge VP størrelse?
</commit_message>
<xml_diff>
--- a/src/csv/temperaturer_kommuner.xlsx
+++ b/src/csv/temperaturer_kommuner.xlsx
@@ -473,10 +473,10 @@
         <v>301</v>
       </c>
       <c r="C2" t="n">
-        <v>-24.79761857</v>
+        <v>-17.62199765</v>
       </c>
       <c r="D2" t="n">
-        <v>28.20133092</v>
+        <v>24.72325618</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
@@ -498,10 +498,10 @@
         <v>1101</v>
       </c>
       <c r="C3" t="n">
-        <v>-14.80984751</v>
+        <v>-9.78755943</v>
       </c>
       <c r="D3" t="n">
-        <v>25.40650675</v>
+        <v>22.65481363</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
@@ -523,10 +523,10 @@
         <v>1103</v>
       </c>
       <c r="C4" t="n">
-        <v>-12.2120653</v>
+        <v>-8.184590181000001</v>
       </c>
       <c r="D4" t="n">
-        <v>26.72558081</v>
+        <v>23.1325692</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
@@ -548,10 +548,10 @@
         <v>1106</v>
       </c>
       <c r="C5" t="n">
-        <v>-11.27313645</v>
+        <v>-7.324116506</v>
       </c>
       <c r="D5" t="n">
-        <v>26.08277079</v>
+        <v>22.47683507</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
@@ -573,10 +573,10 @@
         <v>1108</v>
       </c>
       <c r="C6" t="n">
-        <v>-12.13364261</v>
+        <v>-8.042143703000001</v>
       </c>
       <c r="D6" t="n">
-        <v>26.46333005</v>
+        <v>23.05323796</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
@@ -598,10 +598,10 @@
         <v>1111</v>
       </c>
       <c r="C7" t="n">
-        <v>-15.59439326</v>
+        <v>-10.66660446</v>
       </c>
       <c r="D7" t="n">
-        <v>24.82346111</v>
+        <v>22.67661326</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
@@ -623,10 +623,10 @@
         <v>1112</v>
       </c>
       <c r="C8" t="n">
-        <v>-15.84533613</v>
+        <v>-10.80196909</v>
       </c>
       <c r="D8" t="n">
-        <v>24.93510371</v>
+        <v>22.63701245</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
@@ -648,10 +648,10 @@
         <v>1114</v>
       </c>
       <c r="C9" t="n">
-        <v>-15.01013183</v>
+        <v>-10.37615099</v>
       </c>
       <c r="D9" t="n">
-        <v>25.61112425</v>
+        <v>22.96857134</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -673,10 +673,10 @@
         <v>1119</v>
       </c>
       <c r="C10" t="n">
-        <v>-13.22185467</v>
+        <v>-8.816343857</v>
       </c>
       <c r="D10" t="n">
-        <v>26.00999425</v>
+        <v>22.80107515</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
@@ -698,10 +698,10 @@
         <v>1120</v>
       </c>
       <c r="C11" t="n">
-        <v>-12.74850528</v>
+        <v>-8.392287813999999</v>
       </c>
       <c r="D11" t="n">
-        <v>26.16140629</v>
+        <v>22.99525939</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
@@ -723,10 +723,10 @@
         <v>1121</v>
       </c>
       <c r="C12" t="n">
-        <v>-12.7694284</v>
+        <v>-8.360474364</v>
       </c>
       <c r="D12" t="n">
-        <v>26.14142768</v>
+        <v>22.82829447</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -748,10 +748,10 @@
         <v>1122</v>
       </c>
       <c r="C13" t="n">
-        <v>-14.12266185</v>
+        <v>-9.785195379999999</v>
       </c>
       <c r="D13" t="n">
-        <v>25.72043945</v>
+        <v>23.0034776</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -773,10 +773,10 @@
         <v>1124</v>
       </c>
       <c r="C14" t="n">
-        <v>-12.13238057</v>
+        <v>-8.002704582</v>
       </c>
       <c r="D14" t="n">
-        <v>26.49511065</v>
+        <v>23.06005018</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
@@ -798,10 +798,10 @@
         <v>1127</v>
       </c>
       <c r="C15" t="n">
-        <v>-12.05173395</v>
+        <v>-8.028667883000001</v>
       </c>
       <c r="D15" t="n">
-        <v>26.51449256</v>
+        <v>23.04215559</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
@@ -823,10 +823,10 @@
         <v>1130</v>
       </c>
       <c r="C16" t="n">
-        <v>-13.23964957</v>
+        <v>-8.868242031999999</v>
       </c>
       <c r="D16" t="n">
-        <v>26.72075766</v>
+        <v>23.42009552</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -848,10 +848,10 @@
         <v>1133</v>
       </c>
       <c r="C17" t="n">
-        <v>-13.33657755</v>
+        <v>-9.262662090999999</v>
       </c>
       <c r="D17" t="n">
-        <v>26.46565037</v>
+        <v>23.21835291</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -873,10 +873,10 @@
         <v>1134</v>
       </c>
       <c r="C18" t="n">
-        <v>-15.31889263</v>
+        <v>-10.55259934</v>
       </c>
       <c r="D18" t="n">
-        <v>26.13151125</v>
+        <v>23.17979963</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -898,10 +898,10 @@
         <v>1135</v>
       </c>
       <c r="C19" t="n">
-        <v>-16.59456361</v>
+        <v>-11.38468522</v>
       </c>
       <c r="D19" t="n">
-        <v>26.15811162</v>
+        <v>23.2308921</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
@@ -923,10 +923,10 @@
         <v>1144</v>
       </c>
       <c r="C20" t="n">
-        <v>-11.11602616</v>
+        <v>-7.385177199</v>
       </c>
       <c r="D20" t="n">
-        <v>26.32443508</v>
+        <v>22.74231496</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -948,10 +948,10 @@
         <v>1145</v>
       </c>
       <c r="C21" t="n">
-        <v>-11.95865301</v>
+        <v>-7.986721983</v>
       </c>
       <c r="D21" t="n">
-        <v>25.97977184</v>
+        <v>22.72768379</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -973,10 +973,10 @@
         <v>1146</v>
       </c>
       <c r="C22" t="n">
-        <v>-13.59271298</v>
+        <v>-9.168247526</v>
       </c>
       <c r="D22" t="n">
-        <v>25.66040004</v>
+        <v>22.68509356</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -998,10 +998,10 @@
         <v>1149</v>
       </c>
       <c r="C23" t="n">
-        <v>-11.62340519</v>
+        <v>-7.62532614</v>
       </c>
       <c r="D23" t="n">
-        <v>26.21507231</v>
+        <v>22.60991481</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1023,10 +1023,10 @@
         <v>1151</v>
       </c>
       <c r="C24" t="n">
-        <v>-10.99394787</v>
+        <v>-7.16808655</v>
       </c>
       <c r="D24" t="n">
-        <v>26.01686959</v>
+        <v>22.41902563</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1048,10 +1048,10 @@
         <v>1160</v>
       </c>
       <c r="C25" t="n">
-        <v>-13.11791332</v>
+        <v>-8.314924636000001</v>
       </c>
       <c r="D25" t="n">
-        <v>26.10821433</v>
+        <v>22.85216825</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1073,10 +1073,10 @@
         <v>1505</v>
       </c>
       <c r="C26" t="n">
-        <v>-12.64619997</v>
+        <v>-8.804965409999999</v>
       </c>
       <c r="D26" t="n">
-        <v>25.87679468</v>
+        <v>21.5043386</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -1098,10 +1098,10 @@
         <v>1506</v>
       </c>
       <c r="C27" t="n">
-        <v>-13.5030562</v>
+        <v>-8.355762889999999</v>
       </c>
       <c r="D27" t="n">
-        <v>25.23075512</v>
+        <v>21.51512027</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
@@ -1123,10 +1123,10 @@
         <v>1507</v>
       </c>
       <c r="C28" t="n">
-        <v>-10.89304504</v>
+        <v>-7.38521818</v>
       </c>
       <c r="D28" t="n">
-        <v>25.26935471</v>
+        <v>21.22670588</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -1148,10 +1148,10 @@
         <v>1511</v>
       </c>
       <c r="C29" t="n">
-        <v>-12.35362927</v>
+        <v>-8.871649123999999</v>
       </c>
       <c r="D29" t="n">
-        <v>25.38108917</v>
+        <v>21.66839109</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -1173,10 +1173,10 @@
         <v>1514</v>
       </c>
       <c r="C30" t="n">
-        <v>-13.37096048</v>
+        <v>-9.673758751999999</v>
       </c>
       <c r="D30" t="n">
-        <v>25.50348352</v>
+        <v>22.07791431</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1198,10 +1198,10 @@
         <v>1514</v>
       </c>
       <c r="C31" t="n">
-        <v>-13.37096048</v>
+        <v>-9.673758751999999</v>
       </c>
       <c r="D31" t="n">
-        <v>25.50348352</v>
+        <v>22.07791431</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -1223,10 +1223,10 @@
         <v>1515</v>
       </c>
       <c r="C32" t="n">
-        <v>-10.76875121</v>
+        <v>-7.6661506</v>
       </c>
       <c r="D32" t="n">
-        <v>24.83160142</v>
+        <v>21.27265876</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -1248,10 +1248,10 @@
         <v>1515</v>
       </c>
       <c r="C33" t="n">
-        <v>-10.76875121</v>
+        <v>-7.6661506</v>
       </c>
       <c r="D33" t="n">
-        <v>24.83160142</v>
+        <v>21.27265876</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -1273,10 +1273,10 @@
         <v>1818</v>
       </c>
       <c r="C34" t="n">
-        <v>-14.84673079</v>
+        <v>-10.38856419</v>
       </c>
       <c r="D34" t="n">
-        <v>26.07377252</v>
+        <v>21.9337918</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -1298,10 +1298,10 @@
         <v>1818</v>
       </c>
       <c r="C35" t="n">
-        <v>-14.84673079</v>
+        <v>-10.38856419</v>
       </c>
       <c r="D35" t="n">
-        <v>26.07377252</v>
+        <v>21.9337918</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1323,10 +1323,10 @@
         <v>1516</v>
       </c>
       <c r="C36" t="n">
-        <v>-10.43143858</v>
+        <v>-7.468617479</v>
       </c>
       <c r="D36" t="n">
-        <v>24.92753546</v>
+        <v>21.3818572</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
@@ -1348,10 +1348,10 @@
         <v>1517</v>
       </c>
       <c r="C37" t="n">
-        <v>-11.37378691</v>
+        <v>-8.237844705000001</v>
       </c>
       <c r="D37" t="n">
-        <v>25.7818522</v>
+        <v>21.61987713</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
@@ -1373,10 +1373,10 @@
         <v>1520</v>
       </c>
       <c r="C38" t="n">
-        <v>-14.09936046</v>
+        <v>-9.981369006</v>
       </c>
       <c r="D38" t="n">
-        <v>25.48494432</v>
+        <v>21.93113754</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
@@ -1398,10 +1398,10 @@
         <v>1525</v>
       </c>
       <c r="C39" t="n">
-        <v>-14.59788659</v>
+        <v>-10.20665538</v>
       </c>
       <c r="D39" t="n">
-        <v>25.63657268</v>
+        <v>22.25348439</v>
       </c>
       <c r="E39" t="inlineStr">
         <is>
@@ -1423,10 +1423,10 @@
         <v>1528</v>
       </c>
       <c r="C40" t="n">
-        <v>-12.4100262</v>
+        <v>-8.506950345</v>
       </c>
       <c r="D40" t="n">
-        <v>25.83205326</v>
+        <v>21.85467056</v>
       </c>
       <c r="E40" t="inlineStr">
         <is>
@@ -1448,10 +1448,10 @@
         <v>1531</v>
       </c>
       <c r="C41" t="n">
-        <v>-11.15037998</v>
+        <v>-7.997542795</v>
       </c>
       <c r="D41" t="n">
-        <v>25.95826238</v>
+        <v>21.74867774</v>
       </c>
       <c r="E41" t="inlineStr">
         <is>
@@ -1473,10 +1473,10 @@
         <v>1532</v>
       </c>
       <c r="C42" t="n">
-        <v>-9.68620855</v>
+        <v>-6.635483921</v>
       </c>
       <c r="D42" t="n">
-        <v>24.54802527</v>
+        <v>21.09460055</v>
       </c>
       <c r="E42" t="inlineStr">
         <is>
@@ -1498,10 +1498,10 @@
         <v>1535</v>
       </c>
       <c r="C43" t="n">
-        <v>-12.69816985</v>
+        <v>-8.458775145000001</v>
       </c>
       <c r="D43" t="n">
-        <v>24.91637043</v>
+        <v>21.41037327</v>
       </c>
       <c r="E43" t="inlineStr">
         <is>
@@ -1523,10 +1523,10 @@
         <v>1539</v>
       </c>
       <c r="C44" t="n">
-        <v>-15.38318662</v>
+        <v>-10.55719934</v>
       </c>
       <c r="D44" t="n">
-        <v>25.68585186</v>
+        <v>22.11186179</v>
       </c>
       <c r="E44" t="inlineStr">
         <is>
@@ -1548,10 +1548,10 @@
         <v>1547</v>
       </c>
       <c r="C45" t="n">
-        <v>-11.60681839</v>
+        <v>-7.209143891</v>
       </c>
       <c r="D45" t="n">
-        <v>24.21824686</v>
+        <v>20.96244481</v>
       </c>
       <c r="E45" t="inlineStr">
         <is>
@@ -1573,10 +1573,10 @@
         <v>1554</v>
       </c>
       <c r="C46" t="n">
-        <v>-13.03967894</v>
+        <v>-9.227317628</v>
       </c>
       <c r="D46" t="n">
-        <v>25.97873153</v>
+        <v>21.79424566</v>
       </c>
       <c r="E46" t="inlineStr">
         <is>
@@ -1598,10 +1598,10 @@
         <v>1557</v>
       </c>
       <c r="C47" t="n">
-        <v>-13.88619329</v>
+        <v>-9.545566568</v>
       </c>
       <c r="D47" t="n">
-        <v>25.97821511</v>
+        <v>22.01473853</v>
       </c>
       <c r="E47" t="inlineStr">
         <is>
@@ -1623,10 +1623,10 @@
         <v>1560</v>
       </c>
       <c r="C48" t="n">
-        <v>-16.23149314</v>
+        <v>-11.48648814</v>
       </c>
       <c r="D48" t="n">
-        <v>26.98668699</v>
+        <v>22.72743399</v>
       </c>
       <c r="E48" t="inlineStr">
         <is>
@@ -1648,10 +1648,10 @@
         <v>1563</v>
       </c>
       <c r="C49" t="n">
-        <v>-18.79300481</v>
+        <v>-13.2123682</v>
       </c>
       <c r="D49" t="n">
-        <v>26.81688465</v>
+        <v>22.51096829</v>
       </c>
       <c r="E49" t="inlineStr">
         <is>
@@ -1673,10 +1673,10 @@
         <v>1566</v>
       </c>
       <c r="C50" t="n">
-        <v>-19.11688024</v>
+        <v>-13.47514296</v>
       </c>
       <c r="D50" t="n">
-        <v>27.57487439</v>
+        <v>22.5349706</v>
       </c>
       <c r="E50" t="inlineStr">
         <is>
@@ -1698,10 +1698,10 @@
         <v>1573</v>
       </c>
       <c r="C51" t="n">
-        <v>-12.26270013</v>
+        <v>-8.146319153</v>
       </c>
       <c r="D51" t="n">
-        <v>23.47053235</v>
+        <v>20.25856689</v>
       </c>
       <c r="E51" t="inlineStr">
         <is>
@@ -1723,10 +1723,10 @@
         <v>1576</v>
       </c>
       <c r="C52" t="n">
-        <v>-14.69605527</v>
+        <v>-10.44248742</v>
       </c>
       <c r="D52" t="n">
-        <v>25.14705746</v>
+        <v>21.23339013</v>
       </c>
       <c r="E52" t="inlineStr">
         <is>
@@ -1748,10 +1748,10 @@
         <v>1577</v>
       </c>
       <c r="C53" t="n">
-        <v>-12.5858143</v>
+        <v>-8.673121816</v>
       </c>
       <c r="D53" t="n">
-        <v>25.12537387</v>
+        <v>21.54994938</v>
       </c>
       <c r="E53" t="inlineStr">
         <is>
@@ -1773,10 +1773,10 @@
         <v>1804</v>
       </c>
       <c r="C54" t="n">
-        <v>-14.75215122</v>
+        <v>-11.52527686</v>
       </c>
       <c r="D54" t="n">
-        <v>26.05424347</v>
+        <v>22.21039322</v>
       </c>
       <c r="E54" t="inlineStr">
         <is>
@@ -1798,10 +1798,10 @@
         <v>1806</v>
       </c>
       <c r="C55" t="n">
-        <v>-19.70879364</v>
+        <v>-16.84580261</v>
       </c>
       <c r="D55" t="n">
-        <v>26.84708675</v>
+        <v>22.52445562</v>
       </c>
       <c r="E55" t="inlineStr">
         <is>
@@ -1823,10 +1823,10 @@
         <v>1811</v>
       </c>
       <c r="C56" t="n">
-        <v>-18.99451469</v>
+        <v>-14.46349826</v>
       </c>
       <c r="D56" t="n">
-        <v>27.0183588</v>
+        <v>22.41316708</v>
       </c>
       <c r="E56" t="inlineStr">
         <is>
@@ -1848,10 +1848,10 @@
         <v>1812</v>
       </c>
       <c r="C57" t="n">
-        <v>-16.88559773</v>
+        <v>-13.18366955</v>
       </c>
       <c r="D57" t="n">
-        <v>26.91786905</v>
+        <v>22.46282589</v>
       </c>
       <c r="E57" t="inlineStr">
         <is>
@@ -1873,10 +1873,10 @@
         <v>1813</v>
       </c>
       <c r="C58" t="n">
-        <v>-15.89159951</v>
+        <v>-11.7405827</v>
       </c>
       <c r="D58" t="n">
-        <v>27.04613701</v>
+        <v>22.37709877</v>
       </c>
       <c r="E58" t="inlineStr">
         <is>
@@ -1898,10 +1898,10 @@
         <v>1815</v>
       </c>
       <c r="C59" t="n">
-        <v>-15.12350682</v>
+        <v>-11.42821356</v>
       </c>
       <c r="D59" t="n">
-        <v>27.0409032</v>
+        <v>22.19510793</v>
       </c>
       <c r="E59" t="inlineStr">
         <is>
@@ -1923,10 +1923,10 @@
         <v>1816</v>
       </c>
       <c r="C60" t="n">
-        <v>-15.77283485</v>
+        <v>-11.92529538</v>
       </c>
       <c r="D60" t="n">
-        <v>27.96144772</v>
+        <v>23.33627103</v>
       </c>
       <c r="E60" t="inlineStr">
         <is>
@@ -1948,10 +1948,10 @@
         <v>1820</v>
       </c>
       <c r="C61" t="n">
-        <v>-14.78238099</v>
+        <v>-10.54486317</v>
       </c>
       <c r="D61" t="n">
-        <v>27.12018188</v>
+        <v>22.33664374</v>
       </c>
       <c r="E61" t="inlineStr">
         <is>
@@ -1973,10 +1973,10 @@
         <v>1822</v>
       </c>
       <c r="C62" t="n">
-        <v>-17.22792718</v>
+        <v>-12.92395196</v>
       </c>
       <c r="D62" t="n">
-        <v>25.59563952</v>
+        <v>21.93290692</v>
       </c>
       <c r="E62" t="inlineStr">
         <is>
@@ -1998,10 +1998,10 @@
         <v>1824</v>
       </c>
       <c r="C63" t="n">
-        <v>-19.20770228</v>
+        <v>-15.07253774</v>
       </c>
       <c r="D63" t="n">
-        <v>25.51588389</v>
+        <v>21.98761881</v>
       </c>
       <c r="E63" t="inlineStr">
         <is>
@@ -2023,10 +2023,10 @@
         <v>1825</v>
       </c>
       <c r="C64" t="n">
-        <v>-24.18318611</v>
+        <v>-19.76114345</v>
       </c>
       <c r="D64" t="n">
-        <v>28.37185984</v>
+        <v>23.07625079</v>
       </c>
       <c r="E64" t="inlineStr">
         <is>
@@ -2048,10 +2048,10 @@
         <v>1826</v>
       </c>
       <c r="C65" t="n">
-        <v>-27.42621888</v>
+        <v>-23.13371753</v>
       </c>
       <c r="D65" t="n">
-        <v>27.27536223</v>
+        <v>22.15541746</v>
       </c>
       <c r="E65" t="inlineStr">
         <is>
@@ -2073,10 +2073,10 @@
         <v>1827</v>
       </c>
       <c r="C66" t="n">
-        <v>-14.54651308</v>
+        <v>-10.44375081</v>
       </c>
       <c r="D66" t="n">
-        <v>25.92973818</v>
+        <v>21.79813947</v>
       </c>
       <c r="E66" t="inlineStr">
         <is>
@@ -2098,10 +2098,10 @@
         <v>1828</v>
       </c>
       <c r="C67" t="n">
-        <v>-14.59499708</v>
+        <v>-11.02454956</v>
       </c>
       <c r="D67" t="n">
-        <v>26.43051758</v>
+        <v>21.97534934</v>
       </c>
       <c r="E67" t="inlineStr">
         <is>
@@ -2123,10 +2123,10 @@
         <v>1832</v>
       </c>
       <c r="C68" t="n">
-        <v>-22.66852598</v>
+        <v>-17.67719298</v>
       </c>
       <c r="D68" t="n">
-        <v>25.63709072</v>
+        <v>22.12469894</v>
       </c>
       <c r="E68" t="inlineStr">
         <is>
@@ -2148,10 +2148,10 @@
         <v>1833</v>
       </c>
       <c r="C69" t="n">
-        <v>-18.67307358</v>
+        <v>-15.59484844</v>
       </c>
       <c r="D69" t="n">
-        <v>26.09403256</v>
+        <v>22.21301138</v>
       </c>
       <c r="E69" t="inlineStr">
         <is>
@@ -2173,10 +2173,10 @@
         <v>1834</v>
       </c>
       <c r="C70" t="n">
-        <v>-13.4926514</v>
+        <v>-9.782844927999999</v>
       </c>
       <c r="D70" t="n">
-        <v>25.09844367</v>
+        <v>21.32115472</v>
       </c>
       <c r="E70" t="inlineStr">
         <is>
@@ -2198,10 +2198,10 @@
         <v>1835</v>
       </c>
       <c r="C71" t="n">
-        <v>-13.4926514</v>
+        <v>-9.782844927999999</v>
       </c>
       <c r="D71" t="n">
-        <v>25.09844367</v>
+        <v>21.32115472</v>
       </c>
       <c r="E71" t="inlineStr">
         <is>
@@ -2223,10 +2223,10 @@
         <v>1836</v>
       </c>
       <c r="C72" t="n">
-        <v>-12.77702627</v>
+        <v>-9.570517288</v>
       </c>
       <c r="D72" t="n">
-        <v>24.73111801</v>
+        <v>21.09729249</v>
       </c>
       <c r="E72" t="inlineStr">
         <is>
@@ -2248,10 +2248,10 @@
         <v>1837</v>
       </c>
       <c r="C73" t="n">
-        <v>-13.55917022</v>
+        <v>-10.87532637</v>
       </c>
       <c r="D73" t="n">
-        <v>26.4504124</v>
+        <v>22.56238537</v>
       </c>
       <c r="E73" t="inlineStr">
         <is>
@@ -2273,10 +2273,10 @@
         <v>1838</v>
       </c>
       <c r="C74" t="n">
-        <v>-13.19002543</v>
+        <v>-10.64368076</v>
       </c>
       <c r="D74" t="n">
-        <v>25.76808754</v>
+        <v>21.93878824</v>
       </c>
       <c r="E74" t="inlineStr">
         <is>
@@ -2298,10 +2298,10 @@
         <v>1839</v>
       </c>
       <c r="C75" t="n">
-        <v>-15.98007702</v>
+        <v>-13.64707201</v>
       </c>
       <c r="D75" t="n">
-        <v>26.53965478</v>
+        <v>22.6031584</v>
       </c>
       <c r="E75" t="inlineStr">
         <is>
@@ -2323,10 +2323,10 @@
         <v>1840</v>
       </c>
       <c r="C76" t="n">
-        <v>-18.85522672</v>
+        <v>-16.45783612</v>
       </c>
       <c r="D76" t="n">
-        <v>26.33561211</v>
+        <v>22.21190048</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2348,10 +2348,10 @@
         <v>1841</v>
       </c>
       <c r="C77" t="n">
-        <v>-17.65149471</v>
+        <v>-15.33553961</v>
       </c>
       <c r="D77" t="n">
-        <v>27.05587145</v>
+        <v>22.67459614</v>
       </c>
       <c r="E77" t="inlineStr">
         <is>
@@ -2373,10 +2373,10 @@
         <v>1845</v>
       </c>
       <c r="C78" t="n">
-        <v>-17.16836465</v>
+        <v>-14.83593459</v>
       </c>
       <c r="D78" t="n">
-        <v>26.72769751</v>
+        <v>22.37101608</v>
       </c>
       <c r="E78" t="inlineStr">
         <is>
@@ -2398,10 +2398,10 @@
         <v>1848</v>
       </c>
       <c r="C79" t="n">
-        <v>-14.5048125</v>
+        <v>-11.18727578</v>
       </c>
       <c r="D79" t="n">
-        <v>26.42249187</v>
+        <v>22.39547638</v>
       </c>
       <c r="E79" t="inlineStr">
         <is>
@@ -2423,10 +2423,10 @@
         <v>1851</v>
       </c>
       <c r="C80" t="n">
-        <v>-14.46060641</v>
+        <v>-11.04318621</v>
       </c>
       <c r="D80" t="n">
-        <v>26.85320222</v>
+        <v>22.38193042</v>
       </c>
       <c r="E80" t="inlineStr">
         <is>
@@ -2448,10 +2448,10 @@
         <v>1853</v>
       </c>
       <c r="C81" t="n">
-        <v>-16.99504934</v>
+        <v>-14.11556837</v>
       </c>
       <c r="D81" t="n">
-        <v>25.02645937</v>
+        <v>21.27659358</v>
       </c>
       <c r="E81" t="inlineStr">
         <is>
@@ -2473,10 +2473,10 @@
         <v>1856</v>
       </c>
       <c r="C82" t="n">
-        <v>-12.23099213</v>
+        <v>-7.683567352</v>
       </c>
       <c r="D82" t="n">
-        <v>23.68501302</v>
+        <v>19.65045014</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2498,10 +2498,10 @@
         <v>1857</v>
       </c>
       <c r="C83" t="n">
-        <v>-12.23099213</v>
+        <v>-7.683567352</v>
       </c>
       <c r="D83" t="n">
-        <v>23.68501302</v>
+        <v>19.65045014</v>
       </c>
       <c r="E83" t="inlineStr">
         <is>
@@ -2523,10 +2523,10 @@
         <v>1859</v>
       </c>
       <c r="C84" t="n">
-        <v>-16.38758143</v>
+        <v>-12.60265076</v>
       </c>
       <c r="D84" t="n">
-        <v>24.78213477</v>
+        <v>21.2267792</v>
       </c>
       <c r="E84" t="inlineStr">
         <is>
@@ -2548,10 +2548,10 @@
         <v>1860</v>
       </c>
       <c r="C85" t="n">
-        <v>-12.24347221</v>
+        <v>-8.898879528</v>
       </c>
       <c r="D85" t="n">
-        <v>25.40732266</v>
+        <v>21.41230615</v>
       </c>
       <c r="E85" t="inlineStr">
         <is>
@@ -2573,10 +2573,10 @@
         <v>1865</v>
       </c>
       <c r="C86" t="n">
-        <v>-11.63822825</v>
+        <v>-8.65907352</v>
       </c>
       <c r="D86" t="n">
-        <v>24.54135135</v>
+        <v>21.45484256</v>
       </c>
       <c r="E86" t="inlineStr">
         <is>
@@ -2598,10 +2598,10 @@
         <v>1866</v>
       </c>
       <c r="C87" t="n">
-        <v>-12.09002298</v>
+        <v>-8.859440545</v>
       </c>
       <c r="D87" t="n">
-        <v>24.57080561</v>
+        <v>21.22584342</v>
       </c>
       <c r="E87" t="inlineStr">
         <is>
@@ -2623,10 +2623,10 @@
         <v>1867</v>
       </c>
       <c r="C88" t="n">
-        <v>-12.47928818</v>
+        <v>-9.51609215</v>
       </c>
       <c r="D88" t="n">
-        <v>24.99454421</v>
+        <v>21.29653919</v>
       </c>
       <c r="E88" t="inlineStr">
         <is>
@@ -2648,10 +2648,10 @@
         <v>1867</v>
       </c>
       <c r="C89" t="n">
-        <v>-12.47928818</v>
+        <v>-9.51609215</v>
       </c>
       <c r="D89" t="n">
-        <v>24.99454421</v>
+        <v>21.29653919</v>
       </c>
       <c r="E89" t="inlineStr">
         <is>
@@ -2673,10 +2673,10 @@
         <v>1868</v>
       </c>
       <c r="C90" t="n">
-        <v>-12.77949405</v>
+        <v>-9.878241528</v>
       </c>
       <c r="D90" t="n">
-        <v>24.48296085</v>
+        <v>20.4112598</v>
       </c>
       <c r="E90" t="inlineStr">
         <is>
@@ -2698,10 +2698,10 @@
         <v>1870</v>
       </c>
       <c r="C91" t="n">
-        <v>-13.09692386</v>
+        <v>-9.99609525</v>
       </c>
       <c r="D91" t="n">
-        <v>26.3030631</v>
+        <v>21.68203053</v>
       </c>
       <c r="E91" t="inlineStr">
         <is>
@@ -2723,10 +2723,10 @@
         <v>1871</v>
       </c>
       <c r="C92" t="n">
-        <v>-13.98408605</v>
+        <v>-10.74654604</v>
       </c>
       <c r="D92" t="n">
-        <v>23.34049635</v>
+        <v>19.32535539</v>
       </c>
       <c r="E92" t="inlineStr">
         <is>
@@ -2748,10 +2748,10 @@
         <v>1874</v>
       </c>
       <c r="C93" t="n">
-        <v>-12.38893826</v>
+        <v>-8.713340841999999</v>
       </c>
       <c r="D93" t="n">
-        <v>25.08959961</v>
+        <v>20.92768455</v>
       </c>
       <c r="E93" t="inlineStr">
         <is>
@@ -2773,10 +2773,10 @@
         <v>1875</v>
       </c>
       <c r="C94" t="n">
-        <v>-14.24800727</v>
+        <v>-11.83946052</v>
       </c>
       <c r="D94" t="n">
-        <v>27.61425413</v>
+        <v>23.207709</v>
       </c>
       <c r="E94" t="inlineStr">
         <is>
@@ -2798,10 +2798,10 @@
         <v>3001</v>
       </c>
       <c r="C95" t="n">
-        <v>-22.45228777</v>
+        <v>-15.50568568</v>
       </c>
       <c r="D95" t="n">
-        <v>26.93373032</v>
+        <v>23.88115976</v>
       </c>
       <c r="E95" t="inlineStr">
         <is>
@@ -2823,10 +2823,10 @@
         <v>3002</v>
       </c>
       <c r="C96" t="n">
-        <v>-23.33161201</v>
+        <v>-16.44349659</v>
       </c>
       <c r="D96" t="n">
-        <v>27.22958611</v>
+        <v>24.10203344</v>
       </c>
       <c r="E96" t="inlineStr">
         <is>
@@ -2848,10 +2848,10 @@
         <v>3003</v>
       </c>
       <c r="C97" t="n">
-        <v>-25.06447326</v>
+        <v>-16.96735041</v>
       </c>
       <c r="D97" t="n">
-        <v>27.42374895</v>
+        <v>24.06179522</v>
       </c>
       <c r="E97" t="inlineStr">
         <is>
@@ -2873,10 +2873,10 @@
         <v>3004</v>
       </c>
       <c r="C98" t="n">
-        <v>-22.27098491</v>
+        <v>-15.25196302</v>
       </c>
       <c r="D98" t="n">
-        <v>26.95675854</v>
+        <v>24.01333327</v>
       </c>
       <c r="E98" t="inlineStr">
         <is>
@@ -2898,10 +2898,10 @@
         <v>3005</v>
       </c>
       <c r="C99" t="n">
-        <v>-24.2127067</v>
+        <v>-17.06663874</v>
       </c>
       <c r="D99" t="n">
-        <v>27.3229602</v>
+        <v>24.32995392</v>
       </c>
       <c r="E99" t="inlineStr">
         <is>
@@ -2923,10 +2923,10 @@
         <v>3006</v>
       </c>
       <c r="C100" t="n">
-        <v>-26.74570698</v>
+        <v>-19.08834502</v>
       </c>
       <c r="D100" t="n">
-        <v>27.35037537</v>
+        <v>23.89692619</v>
       </c>
       <c r="E100" t="inlineStr">
         <is>
@@ -2948,10 +2948,10 @@
         <v>3007</v>
       </c>
       <c r="C101" t="n">
-        <v>-26.44915287</v>
+        <v>-19.17645289</v>
       </c>
       <c r="D101" t="n">
-        <v>28.08385258</v>
+        <v>24.5388383</v>
       </c>
       <c r="E101" t="inlineStr">
         <is>
@@ -2973,10 +2973,10 @@
         <v>3011</v>
       </c>
       <c r="C102" t="n">
-        <v>-19.6574896</v>
+        <v>-13.75113563</v>
       </c>
       <c r="D102" t="n">
-        <v>27.00512383</v>
+        <v>23.92661421</v>
       </c>
       <c r="E102" t="inlineStr">
         <is>
@@ -2998,10 +2998,10 @@
         <v>3012</v>
       </c>
       <c r="C103" t="n">
-        <v>-25.94702225</v>
+        <v>-18.18031497</v>
       </c>
       <c r="D103" t="n">
-        <v>26.73965711</v>
+        <v>23.6021007</v>
       </c>
       <c r="E103" t="inlineStr">
         <is>
@@ -3023,10 +3023,10 @@
         <v>3013</v>
       </c>
       <c r="C104" t="n">
-        <v>-29.05741652</v>
+        <v>-20.22441359</v>
       </c>
       <c r="D104" t="n">
-        <v>26.35428244</v>
+        <v>23.49611266</v>
       </c>
       <c r="E104" t="inlineStr">
         <is>
@@ -3048,10 +3048,10 @@
         <v>3015</v>
       </c>
       <c r="C105" t="n">
-        <v>-26.79957911</v>
+        <v>-18.73010703</v>
       </c>
       <c r="D105" t="n">
-        <v>27.0179268</v>
+        <v>23.74761772</v>
       </c>
       <c r="E105" t="inlineStr">
         <is>
@@ -3073,10 +3073,10 @@
         <v>3016</v>
       </c>
       <c r="C106" t="n">
-        <v>-27.00858234</v>
+        <v>-18.91931106</v>
       </c>
       <c r="D106" t="n">
-        <v>27.08260633</v>
+        <v>23.7011112</v>
       </c>
       <c r="E106" t="inlineStr">
         <is>
@@ -3098,10 +3098,10 @@
         <v>3017</v>
       </c>
       <c r="C107" t="n">
-        <v>-24.50083238</v>
+        <v>-16.9581448</v>
       </c>
       <c r="D107" t="n">
-        <v>27.61586602</v>
+        <v>24.24034675</v>
       </c>
       <c r="E107" t="inlineStr">
         <is>
@@ -3123,10 +3123,10 @@
         <v>3018</v>
       </c>
       <c r="C108" t="n">
-        <v>-24.89989121</v>
+        <v>-17.37324279</v>
       </c>
       <c r="D108" t="n">
-        <v>27.64409021</v>
+        <v>24.25382718</v>
       </c>
       <c r="E108" t="inlineStr">
         <is>
@@ -3148,10 +3148,10 @@
         <v>3018</v>
       </c>
       <c r="C109" t="n">
-        <v>-24.89989121</v>
+        <v>-17.37324279</v>
       </c>
       <c r="D109" t="n">
-        <v>27.64409021</v>
+        <v>24.25382718</v>
       </c>
       <c r="E109" t="inlineStr">
         <is>
@@ -3173,10 +3173,10 @@
         <v>3419</v>
       </c>
       <c r="C110" t="n">
-        <v>-32.64393708</v>
+        <v>-24.49591278</v>
       </c>
       <c r="D110" t="n">
-        <v>27.84329047</v>
+        <v>24.0033465</v>
       </c>
       <c r="E110" t="inlineStr">
         <is>
@@ -3198,10 +3198,10 @@
         <v>3419</v>
       </c>
       <c r="C111" t="n">
-        <v>-32.64393708</v>
+        <v>-24.49591278</v>
       </c>
       <c r="D111" t="n">
-        <v>27.84329047</v>
+        <v>24.0033465</v>
       </c>
       <c r="E111" t="inlineStr">
         <is>
@@ -3223,10 +3223,10 @@
         <v>3019</v>
       </c>
       <c r="C112" t="n">
-        <v>-24.36332365</v>
+        <v>-17.45596957</v>
       </c>
       <c r="D112" t="n">
-        <v>27.61107448</v>
+        <v>24.2434275</v>
       </c>
       <c r="E112" t="inlineStr">
         <is>
@@ -3248,10 +3248,10 @@
         <v>3021</v>
       </c>
       <c r="C113" t="n">
-        <v>-24.6386727</v>
+        <v>-17.75080282</v>
       </c>
       <c r="D113" t="n">
-        <v>27.50541965</v>
+        <v>24.24184161</v>
       </c>
       <c r="E113" t="inlineStr">
         <is>
@@ -3273,10 +3273,10 @@
         <v>3022</v>
       </c>
       <c r="C114" t="n">
-        <v>-22.62993848</v>
+        <v>-15.68749243</v>
       </c>
       <c r="D114" t="n">
-        <v>27.32239097</v>
+        <v>24.17660112</v>
       </c>
       <c r="E114" t="inlineStr">
         <is>
@@ -3298,10 +3298,10 @@
         <v>3023</v>
       </c>
       <c r="C115" t="n">
-        <v>-23.92976199</v>
+        <v>-16.91012307</v>
       </c>
       <c r="D115" t="n">
-        <v>27.63714305</v>
+        <v>24.52451577</v>
       </c>
       <c r="E115" t="inlineStr">
         <is>
@@ -3323,10 +3323,10 @@
         <v>3024</v>
       </c>
       <c r="C116" t="n">
-        <v>-23.97461983</v>
+        <v>-17.16505046</v>
       </c>
       <c r="D116" t="n">
-        <v>28.14157509</v>
+        <v>24.82959205</v>
       </c>
       <c r="E116" t="inlineStr">
         <is>
@@ -3348,10 +3348,10 @@
         <v>3025</v>
       </c>
       <c r="C117" t="n">
-        <v>-24.5172191</v>
+        <v>-17.38148039</v>
       </c>
       <c r="D117" t="n">
-        <v>27.82022756</v>
+        <v>24.43334946</v>
       </c>
       <c r="E117" t="inlineStr">
         <is>
@@ -3373,10 +3373,10 @@
         <v>3026</v>
       </c>
       <c r="C118" t="n">
-        <v>-30.92718604</v>
+        <v>-21.82128444</v>
       </c>
       <c r="D118" t="n">
-        <v>26.5712894</v>
+        <v>23.3394629</v>
       </c>
       <c r="E118" t="inlineStr">
         <is>
@@ -3398,10 +3398,10 @@
         <v>3027</v>
       </c>
       <c r="C119" t="n">
-        <v>-26.82562538</v>
+        <v>-19.70654763</v>
       </c>
       <c r="D119" t="n">
-        <v>27.00042397</v>
+        <v>23.64134155</v>
       </c>
       <c r="E119" t="inlineStr">
         <is>
@@ -3423,10 +3423,10 @@
         <v>3028</v>
       </c>
       <c r="C120" t="n">
-        <v>-27.56317769</v>
+        <v>-19.55477822</v>
       </c>
       <c r="D120" t="n">
-        <v>26.73209017</v>
+        <v>23.39609372</v>
       </c>
       <c r="E120" t="inlineStr">
         <is>
@@ -3448,10 +3448,10 @@
         <v>3029</v>
       </c>
       <c r="C121" t="n">
-        <v>-26.32875902</v>
+        <v>-19.12990905</v>
       </c>
       <c r="D121" t="n">
-        <v>27.22280781</v>
+        <v>23.79105291</v>
       </c>
       <c r="E121" t="inlineStr">
         <is>
@@ -3473,10 +3473,10 @@
         <v>3031</v>
       </c>
       <c r="C122" t="n">
-        <v>-26.24364629</v>
+        <v>-19.39265581</v>
       </c>
       <c r="D122" t="n">
-        <v>27.13000087</v>
+        <v>23.64653391</v>
       </c>
       <c r="E122" t="inlineStr">
         <is>
@@ -3498,10 +3498,10 @@
         <v>3032</v>
       </c>
       <c r="C123" t="n">
-        <v>-27.46590097</v>
+        <v>-20.17261821</v>
       </c>
       <c r="D123" t="n">
-        <v>27.30751977</v>
+        <v>23.82410641</v>
       </c>
       <c r="E123" t="inlineStr">
         <is>
@@ -3523,10 +3523,10 @@
         <v>3033</v>
       </c>
       <c r="C124" t="n">
-        <v>-28.55722482</v>
+        <v>-20.7944895</v>
       </c>
       <c r="D124" t="n">
-        <v>27.21299288</v>
+        <v>23.4565275</v>
       </c>
       <c r="E124" t="inlineStr">
         <is>
@@ -3548,10 +3548,10 @@
         <v>3034</v>
       </c>
       <c r="C125" t="n">
-        <v>-30.60587112</v>
+        <v>-22.00724188</v>
       </c>
       <c r="D125" t="n">
-        <v>27.26482762</v>
+        <v>23.60892611</v>
       </c>
       <c r="E125" t="inlineStr">
         <is>
@@ -3573,10 +3573,10 @@
         <v>3034</v>
       </c>
       <c r="C126" t="n">
-        <v>-30.60587112</v>
+        <v>-22.00724188</v>
       </c>
       <c r="D126" t="n">
-        <v>27.26482762</v>
+        <v>23.60892611</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3598,10 +3598,10 @@
         <v>3035</v>
       </c>
       <c r="C127" t="n">
-        <v>-30.24979405</v>
+        <v>-21.74100318</v>
       </c>
       <c r="D127" t="n">
-        <v>27.67467999</v>
+        <v>23.72788966</v>
       </c>
       <c r="E127" t="inlineStr">
         <is>
@@ -3623,10 +3623,10 @@
         <v>3036</v>
       </c>
       <c r="C128" t="n">
-        <v>-28.60235974</v>
+        <v>-20.56994751</v>
       </c>
       <c r="D128" t="n">
-        <v>27.50717721</v>
+        <v>23.61592592</v>
       </c>
       <c r="E128" t="inlineStr">
         <is>
@@ -3648,10 +3648,10 @@
         <v>3037</v>
       </c>
       <c r="C129" t="n">
-        <v>-29.25678109</v>
+        <v>-21.44030637</v>
       </c>
       <c r="D129" t="n">
-        <v>27.4952452</v>
+        <v>23.61758331</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3673,10 +3673,10 @@
         <v>3038</v>
       </c>
       <c r="C130" t="n">
-        <v>-25.14630714</v>
+        <v>-18.30607883</v>
       </c>
       <c r="D130" t="n">
-        <v>28.45302153</v>
+        <v>24.93126208</v>
       </c>
       <c r="E130" t="inlineStr">
         <is>
@@ -3698,10 +3698,10 @@
         <v>3039</v>
       </c>
       <c r="C131" t="n">
-        <v>-30.75568493</v>
+        <v>-22.23147532</v>
       </c>
       <c r="D131" t="n">
-        <v>27.50956161</v>
+        <v>23.81540859</v>
       </c>
       <c r="E131" t="inlineStr">
         <is>
@@ -3723,10 +3723,10 @@
         <v>3041</v>
       </c>
       <c r="C132" t="n">
-        <v>-32.3156373</v>
+        <v>-23.50841716</v>
       </c>
       <c r="D132" t="n">
-        <v>26.46364037</v>
+        <v>23.12194749</v>
       </c>
       <c r="E132" t="inlineStr">
         <is>
@@ -3748,10 +3748,10 @@
         <v>3042</v>
       </c>
       <c r="C133" t="n">
-        <v>-35.32342071</v>
+        <v>-24.41398998</v>
       </c>
       <c r="D133" t="n">
-        <v>24.26767803</v>
+        <v>20.93729493</v>
       </c>
       <c r="E133" t="inlineStr">
         <is>
@@ -3773,10 +3773,10 @@
         <v>3043</v>
       </c>
       <c r="C134" t="n">
-        <v>-32.79472362</v>
+        <v>-23.1976196</v>
       </c>
       <c r="D134" t="n">
-        <v>24.82563261</v>
+        <v>21.66419557</v>
       </c>
       <c r="E134" t="inlineStr">
         <is>
@@ -3798,10 +3798,10 @@
         <v>3044</v>
       </c>
       <c r="C135" t="n">
-        <v>-32.22678239</v>
+        <v>-22.43018422</v>
       </c>
       <c r="D135" t="n">
-        <v>24.24018674</v>
+        <v>21.05769192</v>
       </c>
       <c r="E135" t="inlineStr">
         <is>
@@ -3823,10 +3823,10 @@
         <v>3045</v>
       </c>
       <c r="C136" t="n">
-        <v>-27.39578583</v>
+        <v>-19.67129439</v>
       </c>
       <c r="D136" t="n">
-        <v>27.90347215</v>
+        <v>24.46581383</v>
       </c>
       <c r="E136" t="inlineStr">
         <is>
@@ -3848,10 +3848,10 @@
         <v>3046</v>
       </c>
       <c r="C137" t="n">
-        <v>-28.6879991</v>
+        <v>-20.52237022</v>
       </c>
       <c r="D137" t="n">
-        <v>27.55196239</v>
+        <v>24.12904243</v>
       </c>
       <c r="E137" t="inlineStr">
         <is>
@@ -3873,10 +3873,10 @@
         <v>3047</v>
       </c>
       <c r="C138" t="n">
-        <v>-25.55346535</v>
+        <v>-18.54052399</v>
       </c>
       <c r="D138" t="n">
-        <v>28.22366353</v>
+        <v>24.68624489</v>
       </c>
       <c r="E138" t="inlineStr">
         <is>
@@ -3898,10 +3898,10 @@
         <v>3048</v>
       </c>
       <c r="C139" t="n">
-        <v>-25.0064385</v>
+        <v>-17.8910652</v>
       </c>
       <c r="D139" t="n">
-        <v>27.19956578</v>
+        <v>24.26319828</v>
       </c>
       <c r="E139" t="inlineStr">
         <is>
@@ -3923,10 +3923,10 @@
         <v>3049</v>
       </c>
       <c r="C140" t="n">
-        <v>-24.05882938</v>
+        <v>-17.07801296</v>
       </c>
       <c r="D140" t="n">
-        <v>27.7765878</v>
+        <v>24.48654383</v>
       </c>
       <c r="E140" t="inlineStr">
         <is>
@@ -3948,10 +3948,10 @@
         <v>3050</v>
       </c>
       <c r="C141" t="n">
-        <v>-27.43754856</v>
+        <v>-19.76566493</v>
       </c>
       <c r="D141" t="n">
-        <v>27.11199718</v>
+        <v>23.77541366</v>
       </c>
       <c r="E141" t="inlineStr">
         <is>
@@ -3973,10 +3973,10 @@
         <v>3051</v>
       </c>
       <c r="C142" t="n">
-        <v>-28.6306667</v>
+        <v>-20.605671</v>
       </c>
       <c r="D142" t="n">
-        <v>27.08012645</v>
+        <v>23.53105008</v>
       </c>
       <c r="E142" t="inlineStr">
         <is>
@@ -3998,10 +3998,10 @@
         <v>3052</v>
       </c>
       <c r="C143" t="n">
-        <v>-30.02049864</v>
+        <v>-21.90754827</v>
       </c>
       <c r="D143" t="n">
-        <v>25.58449138</v>
+        <v>22.1957788</v>
       </c>
       <c r="E143" t="inlineStr">
         <is>
@@ -4023,10 +4023,10 @@
         <v>3053</v>
       </c>
       <c r="C144" t="n">
-        <v>-26.72783352</v>
+        <v>-19.78218829</v>
       </c>
       <c r="D144" t="n">
-        <v>28.16259501</v>
+        <v>24.30658027</v>
       </c>
       <c r="E144" t="inlineStr">
         <is>
@@ -4048,10 +4048,10 @@
         <v>3054</v>
       </c>
       <c r="C145" t="n">
-        <v>-27.86395323</v>
+        <v>-19.98299727</v>
       </c>
       <c r="D145" t="n">
-        <v>26.79207386</v>
+        <v>23.22372361</v>
       </c>
       <c r="E145" t="inlineStr">
         <is>
@@ -4073,10 +4073,10 @@
         <v>3401</v>
       </c>
       <c r="C146" t="n">
-        <v>-31.77218649</v>
+        <v>-23.46177948</v>
       </c>
       <c r="D146" t="n">
-        <v>27.53900343</v>
+        <v>23.68409257</v>
       </c>
       <c r="E146" t="inlineStr">
         <is>
@@ -4098,10 +4098,10 @@
         <v>3403</v>
       </c>
       <c r="C147" t="n">
-        <v>-30.51061929</v>
+        <v>-22.31289876</v>
       </c>
       <c r="D147" t="n">
-        <v>27.73881311</v>
+        <v>23.87396393</v>
       </c>
       <c r="E147" t="inlineStr">
         <is>
@@ -4123,10 +4123,10 @@
         <v>3405</v>
       </c>
       <c r="C148" t="n">
-        <v>-32.12918838</v>
+        <v>-22.49086566</v>
       </c>
       <c r="D148" t="n">
-        <v>27.20233521</v>
+        <v>23.41451547</v>
       </c>
       <c r="E148" t="inlineStr">
         <is>
@@ -4148,10 +4148,10 @@
         <v>3407</v>
       </c>
       <c r="C149" t="n">
-        <v>-30.08168775</v>
+        <v>-21.2400122</v>
       </c>
       <c r="D149" t="n">
-        <v>27.57144959</v>
+        <v>23.81705981</v>
       </c>
       <c r="E149" t="inlineStr">
         <is>
@@ -4173,10 +4173,10 @@
         <v>3411</v>
       </c>
       <c r="C150" t="n">
-        <v>-30.6670514</v>
+        <v>-22.19404639</v>
       </c>
       <c r="D150" t="n">
-        <v>27.63016986</v>
+        <v>23.82181521</v>
       </c>
       <c r="E150" t="inlineStr">
         <is>
@@ -4198,10 +4198,10 @@
         <v>3412</v>
       </c>
       <c r="C151" t="n">
-        <v>-32.00205961</v>
+        <v>-23.70634605</v>
       </c>
       <c r="D151" t="n">
-        <v>27.81777506</v>
+        <v>23.85520152</v>
       </c>
       <c r="E151" t="inlineStr">
         <is>
@@ -4223,10 +4223,10 @@
         <v>3413</v>
       </c>
       <c r="C152" t="n">
-        <v>-31.02606417</v>
+        <v>-22.61636666</v>
       </c>
       <c r="D152" t="n">
-        <v>27.79532189</v>
+        <v>23.7383248</v>
       </c>
       <c r="E152" t="inlineStr">
         <is>
@@ -4248,10 +4248,10 @@
         <v>3414</v>
       </c>
       <c r="C153" t="n">
-        <v>-30.87988698</v>
+        <v>-22.64276545</v>
       </c>
       <c r="D153" t="n">
-        <v>27.5986406</v>
+        <v>23.76064591</v>
       </c>
       <c r="E153" t="inlineStr">
         <is>
@@ -4273,10 +4273,10 @@
         <v>3415</v>
       </c>
       <c r="C154" t="n">
-        <v>-31.30575104</v>
+        <v>-22.98800274</v>
       </c>
       <c r="D154" t="n">
-        <v>27.33747974</v>
+        <v>23.71235271</v>
       </c>
       <c r="E154" t="inlineStr">
         <is>
@@ -4298,10 +4298,10 @@
         <v>3416</v>
       </c>
       <c r="C155" t="n">
-        <v>-31.94381094</v>
+        <v>-23.16552849</v>
       </c>
       <c r="D155" t="n">
-        <v>26.87535227</v>
+        <v>23.39437293</v>
       </c>
       <c r="E155" t="inlineStr">
         <is>
@@ -4323,10 +4323,10 @@
         <v>3417</v>
       </c>
       <c r="C156" t="n">
-        <v>-31.65929579</v>
+        <v>-24.0880955</v>
       </c>
       <c r="D156" t="n">
-        <v>27.49539102</v>
+        <v>23.95397418</v>
       </c>
       <c r="E156" t="inlineStr">
         <is>
@@ -4348,10 +4348,10 @@
         <v>3418</v>
       </c>
       <c r="C157" t="n">
-        <v>-32.74719636</v>
+        <v>-24.68714582</v>
       </c>
       <c r="D157" t="n">
-        <v>27.6973668</v>
+        <v>23.97836341</v>
       </c>
       <c r="E157" t="inlineStr">
         <is>
@@ -4373,10 +4373,10 @@
         <v>3420</v>
       </c>
       <c r="C158" t="n">
-        <v>-33.48901182</v>
+        <v>-24.64007721</v>
       </c>
       <c r="D158" t="n">
-        <v>27.8648384</v>
+        <v>23.77724017</v>
       </c>
       <c r="E158" t="inlineStr">
         <is>
@@ -4398,10 +4398,10 @@
         <v>3421</v>
       </c>
       <c r="C159" t="n">
-        <v>-33.97151641</v>
+        <v>-27.79195075</v>
       </c>
       <c r="D159" t="n">
-        <v>26.39335038</v>
+        <v>22.51623029</v>
       </c>
       <c r="E159" t="inlineStr">
         <is>
@@ -4423,10 +4423,10 @@
         <v>3422</v>
       </c>
       <c r="C160" t="n">
-        <v>-33.43976584</v>
+        <v>-25.67447986</v>
       </c>
       <c r="D160" t="n">
-        <v>26.88856437</v>
+        <v>23.2020599</v>
       </c>
       <c r="E160" t="inlineStr">
         <is>
@@ -4448,10 +4448,10 @@
         <v>3423</v>
       </c>
       <c r="C161" t="n">
-        <v>-35.51537078</v>
+        <v>-26.66784604</v>
       </c>
       <c r="D161" t="n">
-        <v>26.45636115</v>
+        <v>22.27306461</v>
       </c>
       <c r="E161" t="inlineStr">
         <is>
@@ -4473,10 +4473,10 @@
         <v>3424</v>
       </c>
       <c r="C162" t="n">
-        <v>-37.97253748</v>
+        <v>-27.50648125</v>
       </c>
       <c r="D162" t="n">
-        <v>26.37223704</v>
+        <v>21.91173741</v>
       </c>
       <c r="E162" t="inlineStr">
         <is>
@@ -4498,10 +4498,10 @@
         <v>3425</v>
       </c>
       <c r="C163" t="n">
-        <v>-38.43283717</v>
+        <v>-28.94569758</v>
       </c>
       <c r="D163" t="n">
-        <v>25.10704846</v>
+        <v>21.08643703</v>
       </c>
       <c r="E163" t="inlineStr">
         <is>
@@ -4523,10 +4523,10 @@
         <v>3426</v>
       </c>
       <c r="C164" t="n">
-        <v>-39.11576982</v>
+        <v>-29.29850932</v>
       </c>
       <c r="D164" t="n">
-        <v>24.60417725</v>
+        <v>20.52500445</v>
       </c>
       <c r="E164" t="inlineStr">
         <is>
@@ -4548,10 +4548,10 @@
         <v>3427</v>
       </c>
       <c r="C165" t="n">
-        <v>-39.2511853</v>
+        <v>-28.91658994</v>
       </c>
       <c r="D165" t="n">
-        <v>24.99430205</v>
+        <v>20.95145471</v>
       </c>
       <c r="E165" t="inlineStr">
         <is>
@@ -4573,10 +4573,10 @@
         <v>3428</v>
       </c>
       <c r="C166" t="n">
-        <v>-39.01164136</v>
+        <v>-28.73625042</v>
       </c>
       <c r="D166" t="n">
-        <v>25.34776969</v>
+        <v>21.09166067</v>
       </c>
       <c r="E166" t="inlineStr">
         <is>
@@ -4598,10 +4598,10 @@
         <v>3429</v>
       </c>
       <c r="C167" t="n">
-        <v>-34.03142021</v>
+        <v>-24.59008043</v>
       </c>
       <c r="D167" t="n">
-        <v>23.26403086</v>
+        <v>19.6282887</v>
       </c>
       <c r="E167" t="inlineStr">
         <is>
@@ -4623,10 +4623,10 @@
         <v>3430</v>
       </c>
       <c r="C168" t="n">
-        <v>-39.21786401</v>
+        <v>-29.16262847</v>
       </c>
       <c r="D168" t="n">
-        <v>24.4156702</v>
+        <v>20.28546931</v>
       </c>
       <c r="E168" t="inlineStr">
         <is>
@@ -4648,10 +4648,10 @@
         <v>3430</v>
       </c>
       <c r="C169" t="n">
-        <v>-39.21786401</v>
+        <v>-29.16262847</v>
       </c>
       <c r="D169" t="n">
-        <v>24.4156702</v>
+        <v>20.28546931</v>
       </c>
       <c r="E169" t="inlineStr">
         <is>
@@ -4673,10 +4673,10 @@
         <v>3431</v>
       </c>
       <c r="C170" t="n">
-        <v>-33.17506877</v>
+        <v>-24.65598727</v>
       </c>
       <c r="D170" t="n">
-        <v>25.48489812</v>
+        <v>21.36520431</v>
       </c>
       <c r="E170" t="inlineStr">
         <is>
@@ -4698,10 +4698,10 @@
         <v>3432</v>
       </c>
       <c r="C171" t="n">
-        <v>-31.0460083</v>
+        <v>-24.00988648</v>
       </c>
       <c r="D171" t="n">
-        <v>24.65378136</v>
+        <v>20.74926972</v>
       </c>
       <c r="E171" t="inlineStr">
         <is>
@@ -4723,10 +4723,10 @@
         <v>3433</v>
       </c>
       <c r="C172" t="n">
-        <v>-29.72696033</v>
+        <v>-21.80913701</v>
       </c>
       <c r="D172" t="n">
-        <v>25.14238109</v>
+        <v>21.51882061</v>
       </c>
       <c r="E172" t="inlineStr">
         <is>
@@ -4748,10 +4748,10 @@
         <v>3434</v>
       </c>
       <c r="C173" t="n">
-        <v>-31.11306875</v>
+        <v>-23.1171374</v>
       </c>
       <c r="D173" t="n">
-        <v>25.49275182</v>
+        <v>21.62513651</v>
       </c>
       <c r="E173" t="inlineStr">
         <is>
@@ -4773,10 +4773,10 @@
         <v>3435</v>
       </c>
       <c r="C174" t="n">
-        <v>-33.72597257</v>
+        <v>-24.02031734</v>
       </c>
       <c r="D174" t="n">
-        <v>26.14479612</v>
+        <v>22.03695969</v>
       </c>
       <c r="E174" t="inlineStr">
         <is>
@@ -4798,10 +4798,10 @@
         <v>3436</v>
       </c>
       <c r="C175" t="n">
-        <v>-32.82314024</v>
+        <v>-23.40986879</v>
       </c>
       <c r="D175" t="n">
-        <v>26.69560648</v>
+        <v>22.65337433</v>
       </c>
       <c r="E175" t="inlineStr">
         <is>
@@ -4823,10 +4823,10 @@
         <v>3437</v>
       </c>
       <c r="C176" t="n">
-        <v>-33.768894</v>
+        <v>-24.43631033</v>
       </c>
       <c r="D176" t="n">
-        <v>26.38840254</v>
+        <v>22.32089127</v>
       </c>
       <c r="E176" t="inlineStr">
         <is>
@@ -4848,10 +4848,10 @@
         <v>3438</v>
       </c>
       <c r="C177" t="n">
-        <v>-33.27283815</v>
+        <v>-24.00027119</v>
       </c>
       <c r="D177" t="n">
-        <v>26.53408015</v>
+        <v>22.46782051</v>
       </c>
       <c r="E177" t="inlineStr">
         <is>
@@ -4873,10 +4873,10 @@
         <v>3439</v>
       </c>
       <c r="C178" t="n">
-        <v>-32.57090389</v>
+        <v>-22.95455238</v>
       </c>
       <c r="D178" t="n">
-        <v>26.59948162</v>
+        <v>22.77673631</v>
       </c>
       <c r="E178" t="inlineStr">
         <is>
@@ -4898,10 +4898,10 @@
         <v>3440</v>
       </c>
       <c r="C179" t="n">
-        <v>-32.00929414</v>
+        <v>-22.78113011</v>
       </c>
       <c r="D179" t="n">
-        <v>26.57619717</v>
+        <v>23.13858622</v>
       </c>
       <c r="E179" t="inlineStr">
         <is>
@@ -4923,10 +4923,10 @@
         <v>3441</v>
       </c>
       <c r="C180" t="n">
-        <v>-32.11205011</v>
+        <v>-22.90422135</v>
       </c>
       <c r="D180" t="n">
-        <v>26.82043501</v>
+        <v>23.18483538</v>
       </c>
       <c r="E180" t="inlineStr">
         <is>
@@ -4948,10 +4948,10 @@
         <v>3442</v>
       </c>
       <c r="C181" t="n">
-        <v>-30.34848903</v>
+        <v>-21.37791312</v>
       </c>
       <c r="D181" t="n">
-        <v>27.76787615</v>
+        <v>23.61319477</v>
       </c>
       <c r="E181" t="inlineStr">
         <is>
@@ -4973,10 +4973,10 @@
         <v>3443</v>
       </c>
       <c r="C182" t="n">
-        <v>-30.20634419</v>
+        <v>-21.65539444</v>
       </c>
       <c r="D182" t="n">
-        <v>27.30132579</v>
+        <v>23.10673324</v>
       </c>
       <c r="E182" t="inlineStr">
         <is>
@@ -4998,10 +4998,10 @@
         <v>3446</v>
       </c>
       <c r="C183" t="n">
-        <v>-28.12513437</v>
+        <v>-20.80061109</v>
       </c>
       <c r="D183" t="n">
-        <v>27.37628073</v>
+        <v>23.46270539</v>
       </c>
       <c r="E183" t="inlineStr">
         <is>
@@ -5023,10 +5023,10 @@
         <v>3447</v>
       </c>
       <c r="C184" t="n">
-        <v>-30.44095855</v>
+        <v>-21.53542821</v>
       </c>
       <c r="D184" t="n">
-        <v>27.57826909</v>
+        <v>23.49730561</v>
       </c>
       <c r="E184" t="inlineStr">
         <is>
@@ -5048,10 +5048,10 @@
         <v>3448</v>
       </c>
       <c r="C185" t="n">
-        <v>-30.95028827</v>
+        <v>-21.60574244</v>
       </c>
       <c r="D185" t="n">
-        <v>27.43726186</v>
+        <v>23.68103236</v>
       </c>
       <c r="E185" t="inlineStr">
         <is>
@@ -5073,10 +5073,10 @@
         <v>3449</v>
       </c>
       <c r="C186" t="n">
-        <v>-32.49670423</v>
+        <v>-23.43794485</v>
       </c>
       <c r="D186" t="n">
-        <v>26.9409374</v>
+        <v>23.33238283</v>
       </c>
       <c r="E186" t="inlineStr">
         <is>
@@ -5098,10 +5098,10 @@
         <v>3450</v>
       </c>
       <c r="C187" t="n">
-        <v>-32.23202165</v>
+        <v>-23.4727192</v>
       </c>
       <c r="D187" t="n">
-        <v>26.89983042</v>
+        <v>22.97772246</v>
       </c>
       <c r="E187" t="inlineStr">
         <is>
@@ -5123,10 +5123,10 @@
         <v>3451</v>
       </c>
       <c r="C188" t="n">
-        <v>-32.76211077</v>
+        <v>-24.41571262</v>
       </c>
       <c r="D188" t="n">
-        <v>26.49726525</v>
+        <v>22.79516485</v>
       </c>
       <c r="E188" t="inlineStr">
         <is>
@@ -5148,10 +5148,10 @@
         <v>3452</v>
       </c>
       <c r="C189" t="n">
-        <v>-32.34517267</v>
+        <v>-23.91245608</v>
       </c>
       <c r="D189" t="n">
-        <v>26.25399743</v>
+        <v>22.68008668</v>
       </c>
       <c r="E189" t="inlineStr">
         <is>
@@ -5173,10 +5173,10 @@
         <v>3453</v>
       </c>
       <c r="C190" t="n">
-        <v>-32.91986552</v>
+        <v>-24.06561704</v>
       </c>
       <c r="D190" t="n">
-        <v>25.34713955</v>
+        <v>21.90471841</v>
       </c>
       <c r="E190" t="inlineStr">
         <is>
@@ -5198,10 +5198,10 @@
         <v>3454</v>
       </c>
       <c r="C191" t="n">
-        <v>-32.2708674</v>
+        <v>-23.28322588</v>
       </c>
       <c r="D191" t="n">
-        <v>24.85235644</v>
+        <v>21.56976325</v>
       </c>
       <c r="E191" t="inlineStr">
         <is>
@@ -5223,10 +5223,10 @@
         <v>3801</v>
       </c>
       <c r="C192" t="n">
-        <v>-23.48704991</v>
+        <v>-16.58704685</v>
       </c>
       <c r="D192" t="n">
-        <v>27.00167531</v>
+        <v>24.06810631</v>
       </c>
       <c r="E192" t="inlineStr">
         <is>
@@ -5248,10 +5248,10 @@
         <v>3802</v>
       </c>
       <c r="C193" t="n">
-        <v>-23.72528661</v>
+        <v>-17.17392843</v>
       </c>
       <c r="D193" t="n">
-        <v>27.28561</v>
+        <v>24.14557268</v>
       </c>
       <c r="E193" t="inlineStr">
         <is>
@@ -5273,10 +5273,10 @@
         <v>3803</v>
       </c>
       <c r="C194" t="n">
-        <v>-22.31257571</v>
+        <v>-15.76052776</v>
       </c>
       <c r="D194" t="n">
-        <v>26.86762457</v>
+        <v>23.91498028</v>
       </c>
       <c r="E194" t="inlineStr">
         <is>
@@ -5298,10 +5298,10 @@
         <v>3804</v>
       </c>
       <c r="C195" t="n">
-        <v>-20.63202743</v>
+        <v>-14.5066604</v>
       </c>
       <c r="D195" t="n">
-        <v>26.56565073</v>
+        <v>23.83413339</v>
       </c>
       <c r="E195" t="inlineStr">
         <is>
@@ -5323,10 +5323,10 @@
         <v>3805</v>
       </c>
       <c r="C196" t="n">
-        <v>-20.55544972</v>
+        <v>-14.14140587</v>
       </c>
       <c r="D196" t="n">
-        <v>26.85189182</v>
+        <v>24.02906883</v>
       </c>
       <c r="E196" t="inlineStr">
         <is>
@@ -5348,10 +5348,10 @@
         <v>3806</v>
       </c>
       <c r="C197" t="n">
-        <v>-20.99702631</v>
+        <v>-14.43919278</v>
       </c>
       <c r="D197" t="n">
-        <v>26.33174952</v>
+        <v>23.57528186</v>
       </c>
       <c r="E197" t="inlineStr">
         <is>
@@ -5373,10 +5373,10 @@
         <v>3807</v>
       </c>
       <c r="C198" t="n">
-        <v>-21.50206277</v>
+        <v>-15.01210223</v>
       </c>
       <c r="D198" t="n">
-        <v>26.19074131</v>
+        <v>23.64258411</v>
       </c>
       <c r="E198" t="inlineStr">
         <is>
@@ -5398,10 +5398,10 @@
         <v>3808</v>
       </c>
       <c r="C199" t="n">
-        <v>-25.65323576</v>
+        <v>-18.02167395</v>
       </c>
       <c r="D199" t="n">
-        <v>26.90021016</v>
+        <v>23.76264883</v>
       </c>
       <c r="E199" t="inlineStr">
         <is>
@@ -5423,10 +5423,10 @@
         <v>3811</v>
       </c>
       <c r="C200" t="n">
-        <v>-21.99282766</v>
+        <v>-15.33217555</v>
       </c>
       <c r="D200" t="n">
-        <v>26.77928558</v>
+        <v>23.90659743</v>
       </c>
       <c r="E200" t="inlineStr">
         <is>
@@ -5448,10 +5448,10 @@
         <v>3812</v>
       </c>
       <c r="C201" t="n">
-        <v>-23.55538426</v>
+        <v>-16.91103563</v>
       </c>
       <c r="D201" t="n">
-        <v>26.86183631</v>
+        <v>23.75262185</v>
       </c>
       <c r="E201" t="inlineStr">
         <is>
@@ -5473,10 +5473,10 @@
         <v>3813</v>
       </c>
       <c r="C202" t="n">
-        <v>-19.10019494</v>
+        <v>-12.9039098</v>
       </c>
       <c r="D202" t="n">
-        <v>26.39415</v>
+        <v>23.70480407</v>
       </c>
       <c r="E202" t="inlineStr">
         <is>
@@ -5498,10 +5498,10 @@
         <v>3814</v>
       </c>
       <c r="C203" t="n">
-        <v>-18.48456612</v>
+        <v>-11.75910923</v>
       </c>
       <c r="D203" t="n">
-        <v>26.13614697</v>
+        <v>23.33720856</v>
       </c>
       <c r="E203" t="inlineStr">
         <is>
@@ -5523,10 +5523,10 @@
         <v>3815</v>
       </c>
       <c r="C204" t="n">
-        <v>-22.66107128</v>
+        <v>-15.68121598</v>
       </c>
       <c r="D204" t="n">
-        <v>26.48580601</v>
+        <v>23.55457277</v>
       </c>
       <c r="E204" t="inlineStr">
         <is>
@@ -5548,10 +5548,10 @@
         <v>3816</v>
       </c>
       <c r="C205" t="n">
-        <v>-22.51472905</v>
+        <v>-15.83337562</v>
       </c>
       <c r="D205" t="n">
-        <v>26.61350306</v>
+        <v>23.56813481</v>
       </c>
       <c r="E205" t="inlineStr">
         <is>
@@ -5573,10 +5573,10 @@
         <v>3818</v>
       </c>
       <c r="C206" t="n">
-        <v>-26.1031748</v>
+        <v>-18.55394695</v>
       </c>
       <c r="D206" t="n">
-        <v>25.13198319</v>
+        <v>22.14628649</v>
       </c>
       <c r="E206" t="inlineStr">
         <is>
@@ -5598,10 +5598,10 @@
         <v>3819</v>
       </c>
       <c r="C207" t="n">
-        <v>-25.37983883</v>
+        <v>-18.12891514</v>
       </c>
       <c r="D207" t="n">
-        <v>27.11844468</v>
+        <v>23.87093195</v>
       </c>
       <c r="E207" t="inlineStr">
         <is>
@@ -5623,10 +5623,10 @@
         <v>3820</v>
       </c>
       <c r="C208" t="n">
-        <v>-23.65906256</v>
+        <v>-16.62954181</v>
       </c>
       <c r="D208" t="n">
-        <v>26.15683512</v>
+        <v>23.39421098</v>
       </c>
       <c r="E208" t="inlineStr">
         <is>
@@ -5648,10 +5648,10 @@
         <v>3821</v>
       </c>
       <c r="C209" t="n">
-        <v>-21.96690761</v>
+        <v>-15.35662193</v>
       </c>
       <c r="D209" t="n">
-        <v>26.1341308</v>
+        <v>23.3752504</v>
       </c>
       <c r="E209" t="inlineStr">
         <is>
@@ -5673,10 +5673,10 @@
         <v>3822</v>
       </c>
       <c r="C210" t="n">
-        <v>-23.39542357</v>
+        <v>-16.42039927</v>
       </c>
       <c r="D210" t="n">
-        <v>25.45405728</v>
+        <v>22.6366077</v>
       </c>
       <c r="E210" t="inlineStr">
         <is>
@@ -5698,10 +5698,10 @@
         <v>3823</v>
       </c>
       <c r="C211" t="n">
-        <v>-22.90374684</v>
+        <v>-16.20618907</v>
       </c>
       <c r="D211" t="n">
-        <v>24.98872256</v>
+        <v>22.46933831</v>
       </c>
       <c r="E211" t="inlineStr">
         <is>
@@ -5723,10 +5723,10 @@
         <v>3824</v>
       </c>
       <c r="C212" t="n">
-        <v>-20.17018347</v>
+        <v>-14.40338046</v>
       </c>
       <c r="D212" t="n">
-        <v>25.67743158</v>
+        <v>23.09122268</v>
       </c>
       <c r="E212" t="inlineStr">
         <is>
@@ -5748,10 +5748,10 @@
         <v>3825</v>
       </c>
       <c r="C213" t="n">
-        <v>-24.30299036</v>
+        <v>-18.56561192</v>
       </c>
       <c r="D213" t="n">
-        <v>23.68081307</v>
+        <v>21.1238109</v>
       </c>
       <c r="E213" t="inlineStr">
         <is>
@@ -5773,10 +5773,10 @@
         <v>4201</v>
       </c>
       <c r="C214" t="n">
-        <v>-19.74979521</v>
+        <v>-12.96414371</v>
       </c>
       <c r="D214" t="n">
-        <v>26.26106748</v>
+        <v>23.25690646</v>
       </c>
       <c r="E214" t="inlineStr">
         <is>
@@ -5798,10 +5798,10 @@
         <v>4202</v>
       </c>
       <c r="C215" t="n">
-        <v>-19.95721481</v>
+        <v>-13.10696435</v>
       </c>
       <c r="D215" t="n">
-        <v>25.81626627</v>
+        <v>23.01136162</v>
       </c>
       <c r="E215" t="inlineStr">
         <is>
@@ -5823,10 +5823,10 @@
         <v>4203</v>
       </c>
       <c r="C216" t="n">
-        <v>-19.74379556</v>
+        <v>-13.03255163</v>
       </c>
       <c r="D216" t="n">
-        <v>25.89611081</v>
+        <v>23.12636789</v>
       </c>
       <c r="E216" t="inlineStr">
         <is>
@@ -5848,10 +5848,10 @@
         <v>4204</v>
       </c>
       <c r="C217" t="n">
-        <v>-18.91424433</v>
+        <v>-11.90245679</v>
       </c>
       <c r="D217" t="n">
-        <v>25.52635704</v>
+        <v>23.0553875</v>
       </c>
       <c r="E217" t="inlineStr">
         <is>
@@ -5873,10 +5873,10 @@
         <v>4205</v>
       </c>
       <c r="C218" t="n">
-        <v>-15.58620432</v>
+        <v>-9.56326402</v>
       </c>
       <c r="D218" t="n">
-        <v>25.42430797</v>
+        <v>22.94828011</v>
       </c>
       <c r="E218" t="inlineStr">
         <is>
@@ -5898,10 +5898,10 @@
         <v>4206</v>
       </c>
       <c r="C219" t="n">
-        <v>-13.54528928</v>
+        <v>-8.762831861</v>
       </c>
       <c r="D219" t="n">
-        <v>25.39042117</v>
+        <v>22.65873388</v>
       </c>
       <c r="E219" t="inlineStr">
         <is>
@@ -5923,10 +5923,10 @@
         <v>4207</v>
       </c>
       <c r="C220" t="n">
-        <v>-15.54760966</v>
+        <v>-10.45927932</v>
       </c>
       <c r="D220" t="n">
-        <v>24.68974774</v>
+        <v>22.74737295</v>
       </c>
       <c r="E220" t="inlineStr">
         <is>
@@ -5948,10 +5948,10 @@
         <v>4211</v>
       </c>
       <c r="C221" t="n">
-        <v>-21.9192348</v>
+        <v>-14.53866691</v>
       </c>
       <c r="D221" t="n">
-        <v>26.75509186</v>
+        <v>23.4654855</v>
       </c>
       <c r="E221" t="inlineStr">
         <is>
@@ -5973,10 +5973,10 @@
         <v>4212</v>
       </c>
       <c r="C222" t="n">
-        <v>-22.92780315</v>
+        <v>-16.23239089</v>
       </c>
       <c r="D222" t="n">
-        <v>26.03824942</v>
+        <v>22.94649054</v>
       </c>
       <c r="E222" t="inlineStr">
         <is>
@@ -5998,10 +5998,10 @@
         <v>4213</v>
       </c>
       <c r="C223" t="n">
-        <v>-21.32293041</v>
+        <v>-14.40836943</v>
       </c>
       <c r="D223" t="n">
-        <v>26.53176153</v>
+        <v>23.31583461</v>
       </c>
       <c r="E223" t="inlineStr">
         <is>
@@ -6023,10 +6023,10 @@
         <v>4214</v>
       </c>
       <c r="C224" t="n">
-        <v>-22.8789906</v>
+        <v>-15.5622875</v>
       </c>
       <c r="D224" t="n">
-        <v>26.58555393</v>
+        <v>23.41164664</v>
       </c>
       <c r="E224" t="inlineStr">
         <is>
@@ -6048,10 +6048,10 @@
         <v>4215</v>
       </c>
       <c r="C225" t="n">
-        <v>-20.1746637</v>
+        <v>-13.00784288</v>
       </c>
       <c r="D225" t="n">
-        <v>25.76831042</v>
+        <v>23.0928321</v>
       </c>
       <c r="E225" t="inlineStr">
         <is>
@@ -6073,10 +6073,10 @@
         <v>4216</v>
       </c>
       <c r="C226" t="n">
-        <v>-21.03540254</v>
+        <v>-14.24839856</v>
       </c>
       <c r="D226" t="n">
-        <v>26.03693138</v>
+        <v>23.38156762</v>
       </c>
       <c r="E226" t="inlineStr">
         <is>
@@ -6098,10 +6098,10 @@
         <v>4217</v>
       </c>
       <c r="C227" t="n">
-        <v>-23.40464247</v>
+        <v>-15.98990273</v>
       </c>
       <c r="D227" t="n">
-        <v>26.31490996</v>
+        <v>23.23441679</v>
       </c>
       <c r="E227" t="inlineStr">
         <is>
@@ -6123,10 +6123,10 @@
         <v>4218</v>
       </c>
       <c r="C228" t="n">
-        <v>-21.40306326</v>
+        <v>-15.27392892</v>
       </c>
       <c r="D228" t="n">
-        <v>25.35793633</v>
+        <v>22.35699728</v>
       </c>
       <c r="E228" t="inlineStr">
         <is>
@@ -6148,10 +6148,10 @@
         <v>4219</v>
       </c>
       <c r="C229" t="n">
-        <v>-21.07351536</v>
+        <v>-14.62284018</v>
       </c>
       <c r="D229" t="n">
-        <v>26.05829355</v>
+        <v>23.08903177</v>
       </c>
       <c r="E229" t="inlineStr">
         <is>
@@ -6173,10 +6173,10 @@
         <v>4220</v>
       </c>
       <c r="C230" t="n">
-        <v>-21.18106318</v>
+        <v>-14.79388904</v>
       </c>
       <c r="D230" t="n">
-        <v>25.59195544</v>
+        <v>22.96912175</v>
       </c>
       <c r="E230" t="inlineStr">
         <is>
@@ -6198,10 +6198,10 @@
         <v>4221</v>
       </c>
       <c r="C231" t="n">
-        <v>-21.75540117</v>
+        <v>-16.15067323</v>
       </c>
       <c r="D231" t="n">
-        <v>24.22406036</v>
+        <v>21.8836752</v>
       </c>
       <c r="E231" t="inlineStr">
         <is>
@@ -6223,10 +6223,10 @@
         <v>4222</v>
       </c>
       <c r="C232" t="n">
-        <v>-29.62546725</v>
+        <v>-22.23370951</v>
       </c>
       <c r="D232" t="n">
-        <v>21.96868612</v>
+        <v>19.08063932</v>
       </c>
       <c r="E232" t="inlineStr">
         <is>
@@ -6248,10 +6248,10 @@
         <v>4223</v>
       </c>
       <c r="C233" t="n">
-        <v>-20.03112337</v>
+        <v>-13.18516519</v>
       </c>
       <c r="D233" t="n">
-        <v>25.78473735</v>
+        <v>23.24161257</v>
       </c>
       <c r="E233" t="inlineStr">
         <is>
@@ -6273,10 +6273,10 @@
         <v>4224</v>
       </c>
       <c r="C234" t="n">
-        <v>-20.05040542</v>
+        <v>-14.63800784</v>
       </c>
       <c r="D234" t="n">
-        <v>24.71089006</v>
+        <v>22.22760523</v>
       </c>
       <c r="E234" t="inlineStr">
         <is>
@@ -6298,10 +6298,10 @@
         <v>4225</v>
       </c>
       <c r="C235" t="n">
-        <v>-14.95083832</v>
+        <v>-9.174150836000001</v>
       </c>
       <c r="D235" t="n">
-        <v>25.1585569</v>
+        <v>22.79776072</v>
       </c>
       <c r="E235" t="inlineStr">
         <is>
@@ -6323,10 +6323,10 @@
         <v>4226</v>
       </c>
       <c r="C236" t="n">
-        <v>-18.1182312</v>
+        <v>-12.53462817</v>
       </c>
       <c r="D236" t="n">
-        <v>24.86785364</v>
+        <v>22.81234477</v>
       </c>
       <c r="E236" t="inlineStr">
         <is>
@@ -6348,10 +6348,10 @@
         <v>4227</v>
       </c>
       <c r="C237" t="n">
-        <v>-15.58110189</v>
+        <v>-9.925760533</v>
       </c>
       <c r="D237" t="n">
-        <v>25.07125858</v>
+        <v>22.69484355</v>
       </c>
       <c r="E237" t="inlineStr">
         <is>
@@ -6373,10 +6373,10 @@
         <v>4228</v>
       </c>
       <c r="C238" t="n">
-        <v>-15.91574327</v>
+        <v>-11.35159211</v>
       </c>
       <c r="D238" t="n">
-        <v>25.40711786</v>
+        <v>22.93667892</v>
       </c>
       <c r="E238" t="inlineStr">
         <is>
@@ -6398,10 +6398,10 @@
         <v>4601</v>
       </c>
       <c r="C239" t="n">
-        <v>-13.06233737</v>
+        <v>-9.259856354</v>
       </c>
       <c r="D239" t="n">
-        <v>26.80133868</v>
+        <v>23.0437098</v>
       </c>
       <c r="E239" t="inlineStr">
         <is>
@@ -6423,10 +6423,10 @@
         <v>4611</v>
       </c>
       <c r="C240" t="n">
-        <v>-14.76592878</v>
+        <v>-9.582378452</v>
       </c>
       <c r="D240" t="n">
-        <v>26.47567861</v>
+        <v>23.13582185</v>
       </c>
       <c r="E240" t="inlineStr">
         <is>
@@ -6448,10 +6448,10 @@
         <v>4612</v>
       </c>
       <c r="C241" t="n">
-        <v>-12.15043744</v>
+        <v>-7.943089961</v>
       </c>
       <c r="D241" t="n">
-        <v>25.96580433</v>
+        <v>22.48617251</v>
       </c>
       <c r="E241" t="inlineStr">
         <is>
@@ -6473,10 +6473,10 @@
         <v>4613</v>
       </c>
       <c r="C242" t="n">
-        <v>-11.00348223</v>
+        <v>-7.138940127</v>
       </c>
       <c r="D242" t="n">
-        <v>26.16810916</v>
+        <v>22.54058356</v>
       </c>
       <c r="E242" t="inlineStr">
         <is>
@@ -6498,10 +6498,10 @@
         <v>4614</v>
       </c>
       <c r="C243" t="n">
-        <v>-12.51739106</v>
+        <v>-8.137589398999999</v>
       </c>
       <c r="D243" t="n">
-        <v>26.14219852</v>
+        <v>22.74587988</v>
       </c>
       <c r="E243" t="inlineStr">
         <is>
@@ -6523,10 +6523,10 @@
         <v>4615</v>
       </c>
       <c r="C244" t="n">
-        <v>-11.99394588</v>
+        <v>-7.831722475</v>
       </c>
       <c r="D244" t="n">
-        <v>25.92118171</v>
+        <v>22.88676601</v>
       </c>
       <c r="E244" t="inlineStr">
         <is>
@@ -6548,10 +6548,10 @@
         <v>4616</v>
       </c>
       <c r="C245" t="n">
-        <v>-13.56567898</v>
+        <v>-9.127959206</v>
       </c>
       <c r="D245" t="n">
-        <v>26.23283509</v>
+        <v>22.87722288</v>
       </c>
       <c r="E245" t="inlineStr">
         <is>
@@ -6573,10 +6573,10 @@
         <v>4617</v>
       </c>
       <c r="C246" t="n">
-        <v>-14.50482392</v>
+        <v>-10.03035855</v>
       </c>
       <c r="D246" t="n">
-        <v>26.38202049</v>
+        <v>23.32703529</v>
       </c>
       <c r="E246" t="inlineStr">
         <is>
@@ -6598,10 +6598,10 @@
         <v>4618</v>
       </c>
       <c r="C247" t="n">
-        <v>-15.6785079</v>
+        <v>-10.85179632</v>
       </c>
       <c r="D247" t="n">
-        <v>26.29851653</v>
+        <v>23.19398836</v>
       </c>
       <c r="E247" t="inlineStr">
         <is>
@@ -6623,10 +6623,10 @@
         <v>4619</v>
       </c>
       <c r="C248" t="n">
-        <v>-17.21309169</v>
+        <v>-12.44506345</v>
       </c>
       <c r="D248" t="n">
-        <v>26.37886265</v>
+        <v>23.09036129</v>
       </c>
       <c r="E248" t="inlineStr">
         <is>
@@ -6648,10 +6648,10 @@
         <v>4620</v>
       </c>
       <c r="C249" t="n">
-        <v>-18.70876277</v>
+        <v>-13.81389992</v>
       </c>
       <c r="D249" t="n">
-        <v>26.9170207</v>
+        <v>23.39808063</v>
       </c>
       <c r="E249" t="inlineStr">
         <is>
@@ -6673,10 +6673,10 @@
         <v>4621</v>
       </c>
       <c r="C250" t="n">
-        <v>-18.89373795</v>
+        <v>-13.5021625</v>
       </c>
       <c r="D250" t="n">
-        <v>26.49745914</v>
+        <v>23.23464977</v>
       </c>
       <c r="E250" t="inlineStr">
         <is>
@@ -6698,10 +6698,10 @@
         <v>4622</v>
       </c>
       <c r="C251" t="n">
-        <v>-15.70026423</v>
+        <v>-11.15010822</v>
       </c>
       <c r="D251" t="n">
-        <v>26.63310494</v>
+        <v>23.12706176</v>
       </c>
       <c r="E251" t="inlineStr">
         <is>
@@ -6723,10 +6723,10 @@
         <v>4623</v>
       </c>
       <c r="C252" t="n">
-        <v>-15.60211318</v>
+        <v>-11.22149388</v>
       </c>
       <c r="D252" t="n">
-        <v>26.73557954</v>
+        <v>23.08708987</v>
       </c>
       <c r="E252" t="inlineStr">
         <is>
@@ -6748,10 +6748,10 @@
         <v>4625</v>
       </c>
       <c r="C253" t="n">
-        <v>-11.12574192</v>
+        <v>-7.334344596</v>
       </c>
       <c r="D253" t="n">
-        <v>26.49481105</v>
+        <v>22.80931041</v>
       </c>
       <c r="E253" t="inlineStr">
         <is>
@@ -6773,10 +6773,10 @@
         <v>4626</v>
       </c>
       <c r="C254" t="n">
-        <v>-11.9143544</v>
+        <v>-7.949048893</v>
       </c>
       <c r="D254" t="n">
-        <v>26.78812785</v>
+        <v>22.81455238</v>
       </c>
       <c r="E254" t="inlineStr">
         <is>
@@ -6798,10 +6798,10 @@
         <v>4627</v>
       </c>
       <c r="C255" t="n">
-        <v>-9.937025258</v>
+        <v>-6.164345189</v>
       </c>
       <c r="D255" t="n">
-        <v>26.95648853</v>
+        <v>22.7478269</v>
       </c>
       <c r="E255" t="inlineStr">
         <is>
@@ -6823,10 +6823,10 @@
         <v>4628</v>
       </c>
       <c r="C256" t="n">
-        <v>-18.1917772</v>
+        <v>-13.95814695</v>
       </c>
       <c r="D256" t="n">
-        <v>25.88870161</v>
+        <v>21.98708269</v>
       </c>
       <c r="E256" t="inlineStr">
         <is>
@@ -6848,10 +6848,10 @@
         <v>4629</v>
       </c>
       <c r="C257" t="n">
-        <v>-15.76860544</v>
+        <v>-11.10280788</v>
       </c>
       <c r="D257" t="n">
-        <v>25.5803477</v>
+        <v>22.14834553</v>
       </c>
       <c r="E257" t="inlineStr">
         <is>
@@ -6873,10 +6873,10 @@
         <v>4630</v>
       </c>
       <c r="C258" t="n">
-        <v>-13.57678895</v>
+        <v>-9.448103753</v>
       </c>
       <c r="D258" t="n">
-        <v>26.48138942</v>
+        <v>22.77272332</v>
       </c>
       <c r="E258" t="inlineStr">
         <is>
@@ -6898,10 +6898,10 @@
         <v>4632</v>
       </c>
       <c r="C259" t="n">
-        <v>-12.02010738</v>
+        <v>-8.043450897</v>
       </c>
       <c r="D259" t="n">
-        <v>26.25899525</v>
+        <v>22.04997992</v>
       </c>
       <c r="E259" t="inlineStr">
         <is>
@@ -6923,10 +6923,10 @@
         <v>4633</v>
       </c>
       <c r="C260" t="n">
-        <v>-11.62644696</v>
+        <v>-7.577420426</v>
       </c>
       <c r="D260" t="n">
-        <v>26.12406548</v>
+        <v>22.0366714</v>
       </c>
       <c r="E260" t="inlineStr">
         <is>
@@ -6948,10 +6948,10 @@
         <v>4634</v>
       </c>
       <c r="C261" t="n">
-        <v>-13.14511494</v>
+        <v>-8.785342759000001</v>
       </c>
       <c r="D261" t="n">
-        <v>26.02481057</v>
+        <v>22.38001617</v>
       </c>
       <c r="E261" t="inlineStr">
         <is>
@@ -6973,10 +6973,10 @@
         <v>4635</v>
       </c>
       <c r="C262" t="n">
-        <v>-12.59028297</v>
+        <v>-8.574457255</v>
       </c>
       <c r="D262" t="n">
-        <v>25.7782825</v>
+        <v>21.90019889</v>
       </c>
       <c r="E262" t="inlineStr">
         <is>
@@ -6998,10 +6998,10 @@
         <v>4636</v>
       </c>
       <c r="C263" t="n">
-        <v>-12.79672579</v>
+        <v>-8.936335517</v>
       </c>
       <c r="D263" t="n">
-        <v>26.2013824</v>
+        <v>22.47902864</v>
       </c>
       <c r="E263" t="inlineStr">
         <is>
@@ -7023,10 +7023,10 @@
         <v>4637</v>
       </c>
       <c r="C264" t="n">
-        <v>-14.5363925</v>
+        <v>-10.16122624</v>
       </c>
       <c r="D264" t="n">
-        <v>26.01434763</v>
+        <v>22.71883283</v>
       </c>
       <c r="E264" t="inlineStr">
         <is>
@@ -7048,10 +7048,10 @@
         <v>4638</v>
       </c>
       <c r="C265" t="n">
-        <v>-19.45637843</v>
+        <v>-13.95362754</v>
       </c>
       <c r="D265" t="n">
-        <v>26.44107261</v>
+        <v>22.67339107</v>
       </c>
       <c r="E265" t="inlineStr">
         <is>
@@ -7073,10 +7073,10 @@
         <v>4639</v>
       </c>
       <c r="C266" t="n">
-        <v>-18.84227338</v>
+        <v>-13.51632529</v>
       </c>
       <c r="D266" t="n">
-        <v>26.11875717</v>
+        <v>22.34581487</v>
       </c>
       <c r="E266" t="inlineStr">
         <is>
@@ -7098,10 +7098,10 @@
         <v>4640</v>
       </c>
       <c r="C267" t="n">
-        <v>-19.97280769</v>
+        <v>-14.68069313</v>
       </c>
       <c r="D267" t="n">
-        <v>26.10087706</v>
+        <v>22.48323844</v>
       </c>
       <c r="E267" t="inlineStr">
         <is>
@@ -7123,10 +7123,10 @@
         <v>4641</v>
       </c>
       <c r="C268" t="n">
-        <v>-19.08639588</v>
+        <v>-13.63350229</v>
       </c>
       <c r="D268" t="n">
-        <v>26.96762473</v>
+        <v>23.39659844</v>
       </c>
       <c r="E268" t="inlineStr">
         <is>
@@ -7148,10 +7148,10 @@
         <v>4642</v>
       </c>
       <c r="C269" t="n">
-        <v>-19.81032721</v>
+        <v>-14.29866026</v>
       </c>
       <c r="D269" t="n">
-        <v>26.85172924</v>
+        <v>23.10272781</v>
       </c>
       <c r="E269" t="inlineStr">
         <is>
@@ -7173,10 +7173,10 @@
         <v>4643</v>
       </c>
       <c r="C270" t="n">
-        <v>-20.71460429</v>
+        <v>-15.6402495</v>
       </c>
       <c r="D270" t="n">
-        <v>26.61482959</v>
+        <v>22.81835201</v>
       </c>
       <c r="E270" t="inlineStr">
         <is>
@@ -7198,10 +7198,10 @@
         <v>4644</v>
       </c>
       <c r="C271" t="n">
-        <v>-19.74481207</v>
+        <v>-14.78185042</v>
       </c>
       <c r="D271" t="n">
-        <v>24.97026274</v>
+        <v>21.69923353</v>
       </c>
       <c r="E271" t="inlineStr">
         <is>
@@ -7223,10 +7223,10 @@
         <v>4645</v>
       </c>
       <c r="C272" t="n">
-        <v>-11.80174178</v>
+        <v>-7.430756974</v>
       </c>
       <c r="D272" t="n">
-        <v>25.36256178</v>
+        <v>21.86727314</v>
       </c>
       <c r="E272" t="inlineStr">
         <is>
@@ -7248,10 +7248,10 @@
         <v>4646</v>
       </c>
       <c r="C273" t="n">
-        <v>-12.627011</v>
+        <v>-8.339231063</v>
       </c>
       <c r="D273" t="n">
-        <v>25.35909887</v>
+        <v>22.16635881</v>
       </c>
       <c r="E273" t="inlineStr">
         <is>
@@ -7273,10 +7273,10 @@
         <v>4648</v>
       </c>
       <c r="C274" t="n">
-        <v>-14.64272942</v>
+        <v>-10.40466215</v>
       </c>
       <c r="D274" t="n">
-        <v>26.26135416</v>
+        <v>22.68719988</v>
       </c>
       <c r="E274" t="inlineStr">
         <is>
@@ -7298,10 +7298,10 @@
         <v>4650</v>
       </c>
       <c r="C275" t="n">
-        <v>-16.56077208</v>
+        <v>-11.92495585</v>
       </c>
       <c r="D275" t="n">
-        <v>25.23720821</v>
+        <v>21.82334708</v>
       </c>
       <c r="E275" t="inlineStr">
         <is>
@@ -7323,10 +7323,10 @@
         <v>4651</v>
       </c>
       <c r="C276" t="n">
-        <v>-16.80469505</v>
+        <v>-12.37889099</v>
       </c>
       <c r="D276" t="n">
-        <v>24.69921299</v>
+        <v>21.73853964</v>
       </c>
       <c r="E276" t="inlineStr">
         <is>
@@ -7348,10 +7348,10 @@
         <v>5001</v>
       </c>
       <c r="C277" t="n">
-        <v>-24.06130938</v>
+        <v>-16.67226536</v>
       </c>
       <c r="D277" t="n">
-        <v>28.03077166</v>
+        <v>23.23267317</v>
       </c>
       <c r="E277" t="inlineStr">
         <is>
@@ -7373,10 +7373,10 @@
         <v>5006</v>
       </c>
       <c r="C278" t="n">
-        <v>-24.01905833</v>
+        <v>-16.97196453</v>
       </c>
       <c r="D278" t="n">
-        <v>28.80642961</v>
+        <v>23.28915061</v>
       </c>
       <c r="E278" t="inlineStr">
         <is>
@@ -7398,10 +7398,10 @@
         <v>5007</v>
       </c>
       <c r="C279" t="n">
-        <v>-21.0491039</v>
+        <v>-14.87195991</v>
       </c>
       <c r="D279" t="n">
-        <v>27.97011365</v>
+        <v>22.73701982</v>
       </c>
       <c r="E279" t="inlineStr">
         <is>
@@ -7423,10 +7423,10 @@
         <v>5014</v>
       </c>
       <c r="C280" t="n">
-        <v>-14.03619227</v>
+        <v>-9.244929061000001</v>
       </c>
       <c r="D280" t="n">
-        <v>24.43346715</v>
+        <v>20.43651919</v>
       </c>
       <c r="E280" t="inlineStr">
         <is>
@@ -7448,10 +7448,10 @@
         <v>5020</v>
       </c>
       <c r="C281" t="n">
-        <v>-19.95885121</v>
+        <v>-13.26415047</v>
       </c>
       <c r="D281" t="n">
-        <v>26.96568087</v>
+        <v>22.45036256</v>
       </c>
       <c r="E281" t="inlineStr">
         <is>
@@ -7473,10 +7473,10 @@
         <v>5021</v>
       </c>
       <c r="C282" t="n">
-        <v>-27.26813614</v>
+        <v>-21.29980516</v>
       </c>
       <c r="D282" t="n">
-        <v>24.94555533</v>
+        <v>20.93836493</v>
       </c>
       <c r="E282" t="inlineStr">
         <is>
@@ -7498,10 +7498,10 @@
         <v>5022</v>
       </c>
       <c r="C283" t="n">
-        <v>-27.14235904</v>
+        <v>-20.47482473</v>
       </c>
       <c r="D283" t="n">
-        <v>25.47938419</v>
+        <v>21.08385241</v>
       </c>
       <c r="E283" t="inlineStr">
         <is>
@@ -7523,10 +7523,10 @@
         <v>5025</v>
       </c>
       <c r="C284" t="n">
-        <v>-37.4986769</v>
+        <v>-28.5940535</v>
       </c>
       <c r="D284" t="n">
-        <v>24.48403483</v>
+        <v>20.15334304</v>
       </c>
       <c r="E284" t="inlineStr">
         <is>
@@ -7548,10 +7548,10 @@
         <v>5026</v>
       </c>
       <c r="C285" t="n">
-        <v>-33.36204169</v>
+        <v>-23.9282225</v>
       </c>
       <c r="D285" t="n">
-        <v>26.00520647</v>
+        <v>21.30990107</v>
       </c>
       <c r="E285" t="inlineStr">
         <is>
@@ -7573,10 +7573,10 @@
         <v>5027</v>
       </c>
       <c r="C286" t="n">
-        <v>-26.89693714</v>
+        <v>-18.47911435</v>
       </c>
       <c r="D286" t="n">
-        <v>27.29209325</v>
+        <v>23.01211708</v>
       </c>
       <c r="E286" t="inlineStr">
         <is>
@@ -7598,10 +7598,10 @@
         <v>5028</v>
       </c>
       <c r="C287" t="n">
-        <v>-25.75713215</v>
+        <v>-17.59987034</v>
       </c>
       <c r="D287" t="n">
-        <v>28.1661187</v>
+        <v>23.29679047</v>
       </c>
       <c r="E287" t="inlineStr">
         <is>
@@ -7623,10 +7623,10 @@
         <v>5029</v>
       </c>
       <c r="C288" t="n">
-        <v>-23.78277158</v>
+        <v>-15.92987564</v>
       </c>
       <c r="D288" t="n">
-        <v>26.57757364</v>
+        <v>22.39188724</v>
       </c>
       <c r="E288" t="inlineStr">
         <is>
@@ -7648,10 +7648,10 @@
         <v>5031</v>
       </c>
       <c r="C289" t="n">
-        <v>-25.4057606</v>
+        <v>-17.22024011</v>
       </c>
       <c r="D289" t="n">
-        <v>28.77925291</v>
+        <v>23.4303167</v>
       </c>
       <c r="E289" t="inlineStr">
         <is>
@@ -7673,10 +7673,10 @@
         <v>5032</v>
       </c>
       <c r="C290" t="n">
-        <v>-28.46787856</v>
+        <v>-19.26104718</v>
       </c>
       <c r="D290" t="n">
-        <v>28.06387356</v>
+        <v>23.22481019</v>
       </c>
       <c r="E290" t="inlineStr">
         <is>
@@ -7698,10 +7698,10 @@
         <v>5033</v>
       </c>
       <c r="C291" t="n">
-        <v>-33.32987212</v>
+        <v>-25.21854887</v>
       </c>
       <c r="D291" t="n">
-        <v>25.42386745</v>
+        <v>20.62624969</v>
       </c>
       <c r="E291" t="inlineStr">
         <is>
@@ -7723,10 +7723,10 @@
         <v>5034</v>
       </c>
       <c r="C292" t="n">
-        <v>-28.49564917</v>
+        <v>-19.24581344</v>
       </c>
       <c r="D292" t="n">
-        <v>28.73019651</v>
+        <v>23.70426977</v>
       </c>
       <c r="E292" t="inlineStr">
         <is>
@@ -7748,10 +7748,10 @@
         <v>5035</v>
       </c>
       <c r="C293" t="n">
-        <v>-25.43339359</v>
+        <v>-17.11082113</v>
       </c>
       <c r="D293" t="n">
-        <v>29.20813603</v>
+        <v>23.55494103</v>
       </c>
       <c r="E293" t="inlineStr">
         <is>
@@ -7773,10 +7773,10 @@
         <v>5036</v>
       </c>
       <c r="C294" t="n">
-        <v>-25.19551272</v>
+        <v>-16.70181801</v>
       </c>
       <c r="D294" t="n">
-        <v>29.69917463</v>
+        <v>24.21311544</v>
       </c>
       <c r="E294" t="inlineStr">
         <is>
@@ -7798,10 +7798,10 @@
         <v>5037</v>
       </c>
       <c r="C295" t="n">
-        <v>-24.06384571</v>
+        <v>-16.79816801</v>
       </c>
       <c r="D295" t="n">
-        <v>28.9976698</v>
+        <v>23.36630224</v>
       </c>
       <c r="E295" t="inlineStr">
         <is>
@@ -7823,10 +7823,10 @@
         <v>5038</v>
       </c>
       <c r="C296" t="n">
-        <v>-24.94651403</v>
+        <v>-17.12418804</v>
       </c>
       <c r="D296" t="n">
-        <v>28.93203427</v>
+        <v>23.38551525</v>
       </c>
       <c r="E296" t="inlineStr">
         <is>
@@ -7848,10 +7848,10 @@
         <v>5041</v>
       </c>
       <c r="C297" t="n">
-        <v>-27.94808197</v>
+        <v>-20.5934417</v>
       </c>
       <c r="D297" t="n">
-        <v>28.73262902</v>
+        <v>23.46485213</v>
       </c>
       <c r="E297" t="inlineStr">
         <is>
@@ -7873,10 +7873,10 @@
         <v>5042</v>
       </c>
       <c r="C298" t="n">
-        <v>-33.86709584</v>
+        <v>-25.48816674</v>
       </c>
       <c r="D298" t="n">
-        <v>26.53545843</v>
+        <v>21.55388229</v>
       </c>
       <c r="E298" t="inlineStr">
         <is>
@@ -7898,10 +7898,10 @@
         <v>5043</v>
       </c>
       <c r="C299" t="n">
-        <v>-33.33500543</v>
+        <v>-25.7625375</v>
       </c>
       <c r="D299" t="n">
-        <v>26.5183322</v>
+        <v>21.25039868</v>
       </c>
       <c r="E299" t="inlineStr">
         <is>
@@ -7923,10 +7923,10 @@
         <v>5044</v>
       </c>
       <c r="C300" t="n">
-        <v>-31.50857028</v>
+        <v>-22.76684233</v>
       </c>
       <c r="D300" t="n">
-        <v>27.9997018</v>
+        <v>22.64337811</v>
       </c>
       <c r="E300" t="inlineStr">
         <is>
@@ -7948,10 +7948,10 @@
         <v>5045</v>
       </c>
       <c r="C301" t="n">
-        <v>-27.45918057</v>
+        <v>-19.73051697</v>
       </c>
       <c r="D301" t="n">
-        <v>28.24553128</v>
+        <v>23.14471355</v>
       </c>
       <c r="E301" t="inlineStr">
         <is>
@@ -7973,10 +7973,10 @@
         <v>5046</v>
       </c>
       <c r="C302" t="n">
-        <v>-26.61345295</v>
+        <v>-18.67810363</v>
       </c>
       <c r="D302" t="n">
-        <v>28.11449409</v>
+        <v>23.08220484</v>
       </c>
       <c r="E302" t="inlineStr">
         <is>
@@ -7998,10 +7998,10 @@
         <v>5047</v>
       </c>
       <c r="C303" t="n">
-        <v>-25.35095164</v>
+        <v>-17.82918741</v>
       </c>
       <c r="D303" t="n">
-        <v>28.18602761</v>
+        <v>22.88607553</v>
       </c>
       <c r="E303" t="inlineStr">
         <is>
@@ -8023,10 +8023,10 @@
         <v>5049</v>
       </c>
       <c r="C304" t="n">
-        <v>-18.41525897</v>
+        <v>-11.64847444</v>
       </c>
       <c r="D304" t="n">
-        <v>26.53403141</v>
+        <v>21.92838057</v>
       </c>
       <c r="E304" t="inlineStr">
         <is>
@@ -8048,10 +8048,10 @@
         <v>5052</v>
       </c>
       <c r="C305" t="n">
-        <v>-17.03007595</v>
+        <v>-12.2273912</v>
       </c>
       <c r="D305" t="n">
-        <v>26.50988727</v>
+        <v>21.95878387</v>
       </c>
       <c r="E305" t="inlineStr">
         <is>
@@ -8073,10 +8073,10 @@
         <v>5053</v>
       </c>
       <c r="C306" t="n">
-        <v>-22.95836842</v>
+        <v>-16.16090407</v>
       </c>
       <c r="D306" t="n">
-        <v>28.60941753</v>
+        <v>22.8799125</v>
       </c>
       <c r="E306" t="inlineStr">
         <is>
@@ -8098,10 +8098,10 @@
         <v>5054</v>
       </c>
       <c r="C307" t="n">
-        <v>-20.47848286</v>
+        <v>-13.87120862</v>
       </c>
       <c r="D307" t="n">
-        <v>27.4280333</v>
+        <v>22.5741771</v>
       </c>
       <c r="E307" t="inlineStr">
         <is>
@@ -8123,10 +8123,10 @@
         <v>5056</v>
       </c>
       <c r="C308" t="n">
-        <v>-15.62918549</v>
+        <v>-10.8012701</v>
       </c>
       <c r="D308" t="n">
-        <v>25.45538477</v>
+        <v>21.21906815</v>
       </c>
       <c r="E308" t="inlineStr">
         <is>
@@ -8148,10 +8148,10 @@
         <v>5057</v>
       </c>
       <c r="C309" t="n">
-        <v>-17.18271391</v>
+        <v>-11.68949409</v>
       </c>
       <c r="D309" t="n">
-        <v>25.99798418</v>
+        <v>21.48237915</v>
       </c>
       <c r="E309" t="inlineStr">
         <is>
@@ -8173,10 +8173,10 @@
         <v>5058</v>
       </c>
       <c r="C310" t="n">
-        <v>-18.42974421</v>
+        <v>-12.00954399</v>
       </c>
       <c r="D310" t="n">
-        <v>27.99100078</v>
+        <v>22.75977133</v>
       </c>
       <c r="E310" t="inlineStr">
         <is>
@@ -8198,10 +8198,10 @@
         <v>5061</v>
       </c>
       <c r="C311" t="n">
-        <v>-22.11518035</v>
+        <v>-15.96968253</v>
       </c>
       <c r="D311" t="n">
-        <v>27.79777911</v>
+        <v>23.09005382</v>
       </c>
       <c r="E311" t="inlineStr">
         <is>
@@ -8223,10 +8223,10 @@
         <v>5401</v>
       </c>
       <c r="C312" t="n">
-        <v>-15.22736183</v>
+        <v>-12.02887323</v>
       </c>
       <c r="D312" t="n">
-        <v>23.71394651</v>
+        <v>19.54039111</v>
       </c>
       <c r="E312" t="inlineStr">
         <is>
@@ -8248,10 +8248,10 @@
         <v>5402</v>
       </c>
       <c r="C313" t="n">
-        <v>-14.9434945</v>
+        <v>-12.05139699</v>
       </c>
       <c r="D313" t="n">
-        <v>24.71925637</v>
+        <v>20.71549602</v>
       </c>
       <c r="E313" t="inlineStr">
         <is>
@@ -8273,10 +8273,10 @@
         <v>5403</v>
       </c>
       <c r="C314" t="n">
-        <v>-30.36072868</v>
+        <v>-23.28188286</v>
       </c>
       <c r="D314" t="n">
-        <v>26.78847295</v>
+        <v>21.87366819</v>
       </c>
       <c r="E314" t="inlineStr">
         <is>
@@ -8298,10 +8298,10 @@
         <v>5404</v>
       </c>
       <c r="C315" t="n">
-        <v>-27.76114086</v>
+        <v>-19.37268018</v>
       </c>
       <c r="D315" t="n">
-        <v>20.84346459</v>
+        <v>17.67053408</v>
       </c>
       <c r="E315" t="inlineStr">
         <is>
@@ -8323,10 +8323,10 @@
         <v>5405</v>
       </c>
       <c r="C316" t="n">
-        <v>-32.24492288</v>
+        <v>-23.41474351</v>
       </c>
       <c r="D316" t="n">
-        <v>22.66273432</v>
+        <v>19.12690682</v>
       </c>
       <c r="E316" t="inlineStr">
         <is>
@@ -8348,10 +8348,10 @@
         <v>5406</v>
       </c>
       <c r="C317" t="n">
-        <v>-27.57403475</v>
+        <v>-17.7708645</v>
       </c>
       <c r="D317" t="n">
-        <v>24.42716369</v>
+        <v>19.69043364</v>
       </c>
       <c r="E317" t="inlineStr">
         <is>
@@ -8373,10 +8373,10 @@
         <v>5411</v>
       </c>
       <c r="C318" t="n">
-        <v>-14.14593174</v>
+        <v>-11.71266045</v>
       </c>
       <c r="D318" t="n">
-        <v>26.1278702</v>
+        <v>21.6670665</v>
       </c>
       <c r="E318" t="inlineStr">
         <is>
@@ -8398,10 +8398,10 @@
         <v>5412</v>
       </c>
       <c r="C319" t="n">
-        <v>-15.8848164</v>
+        <v>-13.25423634</v>
       </c>
       <c r="D319" t="n">
-        <v>26.52947247</v>
+        <v>21.95783697</v>
       </c>
       <c r="E319" t="inlineStr">
         <is>
@@ -8423,10 +8423,10 @@
         <v>5413</v>
       </c>
       <c r="C320" t="n">
-        <v>-18.63038373</v>
+        <v>-15.99870577</v>
       </c>
       <c r="D320" t="n">
-        <v>27.05435732</v>
+        <v>22.38918016</v>
       </c>
       <c r="E320" t="inlineStr">
         <is>
@@ -8448,10 +8448,10 @@
         <v>5414</v>
       </c>
       <c r="C321" t="n">
-        <v>-19.42151943</v>
+        <v>-16.09811557</v>
       </c>
       <c r="D321" t="n">
-        <v>24.94862933</v>
+        <v>21.12368174</v>
       </c>
       <c r="E321" t="inlineStr">
         <is>
@@ -8473,10 +8473,10 @@
         <v>5415</v>
       </c>
       <c r="C322" t="n">
-        <v>-20.77523316</v>
+        <v>-18.01736503</v>
       </c>
       <c r="D322" t="n">
-        <v>25.57240708</v>
+        <v>21.36077008</v>
       </c>
       <c r="E322" t="inlineStr">
         <is>
@@ -8498,10 +8498,10 @@
         <v>5416</v>
       </c>
       <c r="C323" t="n">
-        <v>-25.61623054</v>
+        <v>-21.78028551</v>
       </c>
       <c r="D323" t="n">
-        <v>27.10062673</v>
+        <v>22.24961816</v>
       </c>
       <c r="E323" t="inlineStr">
         <is>
@@ -8523,10 +8523,10 @@
         <v>5417</v>
       </c>
       <c r="C324" t="n">
-        <v>-20.78757787</v>
+        <v>-17.16232746</v>
       </c>
       <c r="D324" t="n">
-        <v>24.83883794</v>
+        <v>20.7586416</v>
       </c>
       <c r="E324" t="inlineStr">
         <is>
@@ -8548,10 +8548,10 @@
         <v>5418</v>
       </c>
       <c r="C325" t="n">
-        <v>-25.0536448</v>
+        <v>-20.18182617</v>
       </c>
       <c r="D325" t="n">
-        <v>25.09264486</v>
+        <v>20.6477476</v>
       </c>
       <c r="E325" t="inlineStr">
         <is>
@@ -8573,10 +8573,10 @@
         <v>5419</v>
       </c>
       <c r="C326" t="n">
-        <v>-23.12339227</v>
+        <v>-18.2749562</v>
       </c>
       <c r="D326" t="n">
-        <v>25.08753006</v>
+        <v>20.46110031</v>
       </c>
       <c r="E326" t="inlineStr">
         <is>
@@ -8598,10 +8598,10 @@
         <v>5420</v>
       </c>
       <c r="C327" t="n">
-        <v>-21.73553528</v>
+        <v>-17.24553208</v>
       </c>
       <c r="D327" t="n">
-        <v>25.12734491</v>
+        <v>20.59204689</v>
       </c>
       <c r="E327" t="inlineStr">
         <is>
@@ -8623,10 +8623,10 @@
         <v>5422</v>
       </c>
       <c r="C328" t="n">
-        <v>-22.43810698</v>
+        <v>-18.79528206</v>
       </c>
       <c r="D328" t="n">
-        <v>24.82364649</v>
+        <v>20.2890482</v>
       </c>
       <c r="E328" t="inlineStr">
         <is>
@@ -8648,10 +8648,10 @@
         <v>5423</v>
       </c>
       <c r="C329" t="n">
-        <v>-13.47044257</v>
+        <v>-10.23793818</v>
       </c>
       <c r="D329" t="n">
-        <v>24.14131641</v>
+        <v>19.47177012</v>
       </c>
       <c r="E329" t="inlineStr">
         <is>
@@ -8673,10 +8673,10 @@
         <v>5424</v>
       </c>
       <c r="C330" t="n">
-        <v>-19.73398086</v>
+        <v>-16.82804056</v>
       </c>
       <c r="D330" t="n">
-        <v>25.06820015</v>
+        <v>20.28034709</v>
       </c>
       <c r="E330" t="inlineStr">
         <is>
@@ -8698,10 +8698,10 @@
         <v>5425</v>
       </c>
       <c r="C331" t="n">
-        <v>-23.21801196</v>
+        <v>-19.62358136</v>
       </c>
       <c r="D331" t="n">
-        <v>25.09589286</v>
+        <v>20.46533226</v>
       </c>
       <c r="E331" t="inlineStr">
         <is>
@@ -8723,10 +8723,10 @@
         <v>5426</v>
       </c>
       <c r="C332" t="n">
-        <v>-20.60030958</v>
+        <v>-17.74012439</v>
       </c>
       <c r="D332" t="n">
-        <v>25.2282637</v>
+        <v>20.56720992</v>
       </c>
       <c r="E332" t="inlineStr">
         <is>
@@ -8748,10 +8748,10 @@
         <v>5427</v>
       </c>
       <c r="C333" t="n">
-        <v>-17.59814373</v>
+        <v>-14.20384979</v>
       </c>
       <c r="D333" t="n">
-        <v>24.70484352</v>
+        <v>19.9468688</v>
       </c>
       <c r="E333" t="inlineStr">
         <is>
@@ -8773,10 +8773,10 @@
         <v>5428</v>
       </c>
       <c r="C334" t="n">
-        <v>-22.04021987</v>
+        <v>-18.17816147</v>
       </c>
       <c r="D334" t="n">
-        <v>25.72434366</v>
+        <v>20.63431763</v>
       </c>
       <c r="E334" t="inlineStr">
         <is>
@@ -8798,10 +8798,10 @@
         <v>5429</v>
       </c>
       <c r="C335" t="n">
-        <v>-23.15046741</v>
+        <v>-17.59484959</v>
       </c>
       <c r="D335" t="n">
-        <v>25.75575504</v>
+        <v>20.79371197</v>
       </c>
       <c r="E335" t="inlineStr">
         <is>
@@ -8823,10 +8823,10 @@
         <v>5430</v>
       </c>
       <c r="C336" t="n">
-        <v>-45.48866845</v>
+        <v>-36.80499422</v>
       </c>
       <c r="D336" t="n">
-        <v>25.31698119</v>
+        <v>21.29590614</v>
       </c>
       <c r="E336" t="inlineStr">
         <is>
@@ -8848,10 +8848,10 @@
         <v>5432</v>
       </c>
       <c r="C337" t="n">
-        <v>-21.02300582</v>
+        <v>-15.46673909</v>
       </c>
       <c r="D337" t="n">
-        <v>24.6486293</v>
+        <v>20.00469586</v>
       </c>
       <c r="E337" t="inlineStr">
         <is>
@@ -8873,10 +8873,10 @@
         <v>5433</v>
       </c>
       <c r="C338" t="n">
-        <v>-25.08504344</v>
+        <v>-16.03281894</v>
       </c>
       <c r="D338" t="n">
-        <v>24.71742562</v>
+        <v>20.08601051</v>
       </c>
       <c r="E338" t="inlineStr">
         <is>
@@ -8898,10 +8898,10 @@
         <v>5434</v>
       </c>
       <c r="C339" t="n">
-        <v>-32.56484098</v>
+        <v>-19.16046995</v>
       </c>
       <c r="D339" t="n">
-        <v>25.36129067</v>
+        <v>19.62790816</v>
       </c>
       <c r="E339" t="inlineStr">
         <is>
@@ -8923,10 +8923,10 @@
         <v>5435</v>
       </c>
       <c r="C340" t="n">
-        <v>-32.24475867</v>
+        <v>-19.17789754</v>
       </c>
       <c r="D340" t="n">
-        <v>25.52097156</v>
+        <v>20.15853093</v>
       </c>
       <c r="E340" t="inlineStr">
         <is>
@@ -8948,10 +8948,10 @@
         <v>5436</v>
       </c>
       <c r="C341" t="n">
-        <v>-37.96250265</v>
+        <v>-28.05696534</v>
       </c>
       <c r="D341" t="n">
-        <v>26.72112819</v>
+        <v>21.12238157</v>
       </c>
       <c r="E341" t="inlineStr">
         <is>
@@ -8973,10 +8973,10 @@
         <v>5437</v>
       </c>
       <c r="C342" t="n">
-        <v>-48.42743495</v>
+        <v>-37.89725583</v>
       </c>
       <c r="D342" t="n">
-        <v>27.21271022</v>
+        <v>22.49416307</v>
       </c>
       <c r="E342" t="inlineStr">
         <is>
@@ -8998,10 +8998,10 @@
         <v>5438</v>
       </c>
       <c r="C343" t="n">
-        <v>-31.20705645</v>
+        <v>-19.40067648</v>
       </c>
       <c r="D343" t="n">
-        <v>24.85648794</v>
+        <v>21.03813906</v>
       </c>
       <c r="E343" t="inlineStr">
         <is>
@@ -9023,10 +9023,10 @@
         <v>5439</v>
       </c>
       <c r="C344" t="n">
-        <v>-29.56625724</v>
+        <v>-17.93155409</v>
       </c>
       <c r="D344" t="n">
-        <v>22.35903977</v>
+        <v>18.64243371</v>
       </c>
       <c r="E344" t="inlineStr">
         <is>
@@ -9048,10 +9048,10 @@
         <v>5440</v>
       </c>
       <c r="C345" t="n">
-        <v>-24.32230663</v>
+        <v>-16.24974659</v>
       </c>
       <c r="D345" t="n">
-        <v>21.85815586</v>
+        <v>18.85653802</v>
       </c>
       <c r="E345" t="inlineStr">
         <is>
@@ -9073,10 +9073,10 @@
         <v>5441</v>
       </c>
       <c r="C346" t="n">
-        <v>-36.33031444</v>
+        <v>-27.76010888</v>
       </c>
       <c r="D346" t="n">
-        <v>24.31116576</v>
+        <v>20.04425162</v>
       </c>
       <c r="E346" t="inlineStr">
         <is>
@@ -9098,10 +9098,10 @@
         <v>5442</v>
       </c>
       <c r="C347" t="n">
-        <v>-36.04809071</v>
+        <v>-27.26131031</v>
       </c>
       <c r="D347" t="n">
-        <v>25.95086045</v>
+        <v>20.71597717</v>
       </c>
       <c r="E347" t="inlineStr">
         <is>
@@ -9123,10 +9123,10 @@
         <v>5443</v>
       </c>
       <c r="C348" t="n">
-        <v>-24.17303433</v>
+        <v>-16.41406891</v>
       </c>
       <c r="D348" t="n">
-        <v>21.94724358</v>
+        <v>18.75515223</v>
       </c>
       <c r="E348" t="inlineStr">
         <is>
@@ -9148,10 +9148,10 @@
         <v>5444</v>
       </c>
       <c r="C349" t="n">
-        <v>-37.82923882</v>
+        <v>-28.6226069</v>
       </c>
       <c r="D349" t="n">
-        <v>26.64092534</v>
+        <v>21.19942557</v>
       </c>
       <c r="E349" t="inlineStr">
         <is>

</xml_diff>